<commit_message>
Added core methods to bitwise_*
</commit_message>
<xml_diff>
--- a/src/wrapped_functions_c++.xlsx
+++ b/src/wrapped_functions_c++.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="4" r:id="rId1"/>
@@ -38,9 +38,6 @@
     <t>bool setBreakOnError(bool flag);</t>
   </si>
   <si>
-    <t>ErrorCallback redirectError( ErrorCallback errCallback,</t>
-  </si>
-  <si>
     <t>void glob(String pattern, std::vector&lt;String&gt;&amp; result, bool recursive = false);</t>
   </si>
   <si>
@@ -760,6 +757,10 @@
   </si>
   <si>
     <t>module</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ErrorCallback redirectError( ErrorCallback errCallback,</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1180,7 +1181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
@@ -1194,24 +1195,24 @@
   <sheetData>
     <row r="2" spans="2:6">
       <c r="B2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E2" t="s">
         <v>167</v>
       </c>
-      <c r="D2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E2" t="s">
-        <v>168</v>
-      </c>
       <c r="F2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C3">
         <f>ROWS(テーブル1[Wrapped])</f>
@@ -1244,9 +1245,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:D238"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A70" sqref="A70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1258,13 +1259,13 @@
   <sheetData>
     <row r="1" spans="2:4">
       <c r="B1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" t="s">
         <v>163</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="2" spans="2:4">
@@ -1320,7 +1321,7 @@
         <v>209</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="2:4">
@@ -1328,7 +1329,7 @@
         <v>231</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:4">
@@ -1336,7 +1337,7 @@
         <v>233</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
@@ -1347,7 +1348,7 @@
         <v>234</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
@@ -1358,7 +1359,7 @@
         <v>235</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
@@ -1369,7 +1370,7 @@
         <v>237</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -1380,7 +1381,7 @@
         <v>247</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -1391,7 +1392,7 @@
         <v>261</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
@@ -1402,7 +1403,7 @@
         <v>271</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
@@ -1413,7 +1414,7 @@
         <v>292</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
@@ -1424,7 +1425,7 @@
         <v>295</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
@@ -1435,7 +1436,7 @@
         <v>307</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
@@ -1446,7 +1447,7 @@
         <v>315</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
@@ -1457,7 +1458,7 @@
         <v>358</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
@@ -1468,7 +1469,7 @@
         <v>365</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
@@ -1479,7 +1480,7 @@
         <v>969</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="2:4">
@@ -1487,7 +1488,7 @@
         <v>1453</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="2:4">
@@ -1495,7 +1496,7 @@
         <v>2120</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="2:4">
@@ -1503,7 +1504,7 @@
         <v>2121</v>
       </c>
       <c r="C26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="2:4">
@@ -1511,7 +1512,7 @@
         <v>2122</v>
       </c>
       <c r="C27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="2:4">
@@ -1519,7 +1520,7 @@
         <v>2125</v>
       </c>
       <c r="C28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="2:4">
@@ -1527,7 +1528,7 @@
         <v>2128</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D29" s="1">
         <v>1</v>
@@ -1538,7 +1539,7 @@
         <v>2131</v>
       </c>
       <c r="C30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D30" s="1">
         <v>1</v>
@@ -1549,7 +1550,7 @@
         <v>2133</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D31" s="1">
         <v>1</v>
@@ -1560,7 +1561,7 @@
         <v>2136</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D32" s="1">
         <v>1</v>
@@ -1571,7 +1572,7 @@
         <v>2139</v>
       </c>
       <c r="C33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D33" s="1">
         <v>1</v>
@@ -1582,7 +1583,7 @@
         <v>2143</v>
       </c>
       <c r="C34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D34" s="1">
         <v>1</v>
@@ -1593,7 +1594,7 @@
         <v>2147</v>
       </c>
       <c r="C35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D35" s="1">
         <v>1</v>
@@ -1604,7 +1605,7 @@
         <v>2151</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D36" s="1">
         <v>1</v>
@@ -1615,7 +1616,7 @@
         <v>2155</v>
       </c>
       <c r="C37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D37" s="1">
         <v>1</v>
@@ -1626,7 +1627,7 @@
         <v>2158</v>
       </c>
       <c r="C38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D38" s="1">
         <v>1</v>
@@ -1637,7 +1638,7 @@
         <v>2162</v>
       </c>
       <c r="C39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D39" s="1">
         <v>1</v>
@@ -1648,7 +1649,7 @@
         <v>2165</v>
       </c>
       <c r="C40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D40" s="1">
         <v>1</v>
@@ -1659,7 +1660,7 @@
         <v>2169</v>
       </c>
       <c r="C41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D41" s="1">
         <v>1</v>
@@ -1670,7 +1671,7 @@
         <v>2171</v>
       </c>
       <c r="C42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D42" s="1">
         <v>1</v>
@@ -1681,7 +1682,7 @@
         <v>2173</v>
       </c>
       <c r="C43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D43" s="1">
         <v>1</v>
@@ -1692,7 +1693,7 @@
         <v>2176</v>
       </c>
       <c r="C44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D44" s="1">
         <v>1</v>
@@ -1703,7 +1704,7 @@
         <v>2178</v>
       </c>
       <c r="C45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D45" s="1">
         <v>1</v>
@@ -1714,7 +1715,7 @@
         <v>2181</v>
       </c>
       <c r="C46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D46" s="1">
         <v>1</v>
@@ -1725,7 +1726,7 @@
         <v>2183</v>
       </c>
       <c r="C47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D47" s="1">
         <v>1</v>
@@ -1736,7 +1737,7 @@
         <v>2187</v>
       </c>
       <c r="C48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D48" s="1">
         <v>1</v>
@@ -1747,7 +1748,7 @@
         <v>2194</v>
       </c>
       <c r="C49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D49" s="1">
         <v>1</v>
@@ -1758,7 +1759,7 @@
         <v>2198</v>
       </c>
       <c r="C50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D50" s="1">
         <v>1</v>
@@ -1769,7 +1770,7 @@
         <v>2201</v>
       </c>
       <c r="C51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D51" s="1">
         <v>1</v>
@@ -1780,7 +1781,7 @@
         <v>2205</v>
       </c>
       <c r="C52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="2:4">
@@ -1788,7 +1789,7 @@
         <v>2208</v>
       </c>
       <c r="C53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="2:4">
@@ -1796,7 +1797,7 @@
         <v>2209</v>
       </c>
       <c r="C54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="2:4">
@@ -1804,7 +1805,7 @@
         <v>2212</v>
       </c>
       <c r="C55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56" spans="2:4">
@@ -1812,7 +1813,7 @@
         <v>2215</v>
       </c>
       <c r="C56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="2:4">
@@ -1820,7 +1821,7 @@
         <v>2216</v>
       </c>
       <c r="C57" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="2:4">
@@ -1828,7 +1829,7 @@
         <v>2219</v>
       </c>
       <c r="C58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="2:4">
@@ -1836,7 +1837,7 @@
         <v>2222</v>
       </c>
       <c r="C59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="2:4">
@@ -1844,7 +1845,7 @@
         <v>2224</v>
       </c>
       <c r="C60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="2:4">
@@ -1852,7 +1853,7 @@
         <v>2226</v>
       </c>
       <c r="C61" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="2:4">
@@ -1860,7 +1861,7 @@
         <v>2230</v>
       </c>
       <c r="C62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" spans="2:4">
@@ -1868,7 +1869,7 @@
         <v>2233</v>
       </c>
       <c r="C63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" spans="2:4">
@@ -1876,7 +1877,7 @@
         <v>2236</v>
       </c>
       <c r="C64" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="65" spans="2:3">
@@ -1884,7 +1885,7 @@
         <v>2239</v>
       </c>
       <c r="C65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="66" spans="2:3">
@@ -1892,7 +1893,7 @@
         <v>2240</v>
       </c>
       <c r="C66" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" spans="2:3">
@@ -1900,7 +1901,7 @@
         <v>2242</v>
       </c>
       <c r="C67" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" spans="2:3">
@@ -1908,7 +1909,7 @@
         <v>2243</v>
       </c>
       <c r="C68" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="69" spans="2:3">
@@ -1916,7 +1917,7 @@
         <v>2244</v>
       </c>
       <c r="C69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="70" spans="2:3">
@@ -1924,7 +1925,7 @@
         <v>2246</v>
       </c>
       <c r="C70" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="71" spans="2:3">
@@ -1932,7 +1933,7 @@
         <v>2247</v>
       </c>
       <c r="C71" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="72" spans="2:3">
@@ -1940,7 +1941,7 @@
         <v>2248</v>
       </c>
       <c r="C72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="2:3">
@@ -1948,7 +1949,7 @@
         <v>2251</v>
       </c>
       <c r="C73" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="74" spans="2:3">
@@ -1956,7 +1957,7 @@
         <v>2254</v>
       </c>
       <c r="C74" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="75" spans="2:3">
@@ -1964,7 +1965,7 @@
         <v>2257</v>
       </c>
       <c r="C75" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="76" spans="2:3">
@@ -1972,7 +1973,7 @@
         <v>2260</v>
       </c>
       <c r="C76" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="77" spans="2:3">
@@ -1980,7 +1981,7 @@
         <v>2263</v>
       </c>
       <c r="C77" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="78" spans="2:3">
@@ -1988,7 +1989,7 @@
         <v>2265</v>
       </c>
       <c r="C78" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="79" spans="2:3">
@@ -1996,7 +1997,7 @@
         <v>2268</v>
       </c>
       <c r="C79" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="80" spans="2:3">
@@ -2004,7 +2005,7 @@
         <v>2270</v>
       </c>
       <c r="C80" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="81" spans="2:3">
@@ -2012,7 +2013,7 @@
         <v>2272</v>
       </c>
       <c r="C81" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="82" spans="2:3">
@@ -2020,7 +2021,7 @@
         <v>2275</v>
       </c>
       <c r="C82" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="83" spans="2:3">
@@ -2028,7 +2029,7 @@
         <v>2277</v>
       </c>
       <c r="C83" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="84" spans="2:3">
@@ -2036,7 +2037,7 @@
         <v>2279</v>
       </c>
       <c r="C84" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="85" spans="2:3">
@@ -2044,7 +2045,7 @@
         <v>2281</v>
       </c>
       <c r="C85" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="86" spans="2:3">
@@ -2052,7 +2053,7 @@
         <v>2284</v>
       </c>
       <c r="C86" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="87" spans="2:3">
@@ -2060,7 +2061,7 @@
         <v>2286</v>
       </c>
       <c r="C87" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="88" spans="2:3">
@@ -2068,7 +2069,7 @@
         <v>2288</v>
       </c>
       <c r="C88" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="89" spans="2:3">
@@ -2076,7 +2077,7 @@
         <v>2290</v>
       </c>
       <c r="C89" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="90" spans="2:3">
@@ -2084,7 +2085,7 @@
         <v>2292</v>
       </c>
       <c r="C90" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="91" spans="2:3">
@@ -2092,7 +2093,7 @@
         <v>2294</v>
       </c>
       <c r="C91" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="92" spans="2:3">
@@ -2100,7 +2101,7 @@
         <v>2296</v>
       </c>
       <c r="C92" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="93" spans="2:3">
@@ -2108,7 +2109,7 @@
         <v>2297</v>
       </c>
       <c r="C93" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="94" spans="2:3">
@@ -2116,7 +2117,7 @@
         <v>2298</v>
       </c>
       <c r="C94" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="95" spans="2:3">
@@ -2124,7 +2125,7 @@
         <v>2299</v>
       </c>
       <c r="C95" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="96" spans="2:3">
@@ -2132,7 +2133,7 @@
         <v>2302</v>
       </c>
       <c r="C96" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="97" spans="2:3">
@@ -2140,7 +2141,7 @@
         <v>2305</v>
       </c>
       <c r="C97" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="98" spans="2:3">
@@ -2148,7 +2149,7 @@
         <v>2309</v>
       </c>
       <c r="C98" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="99" spans="2:3">
@@ -2156,7 +2157,7 @@
         <v>2312</v>
       </c>
       <c r="C99" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="100" spans="2:3">
@@ -2164,7 +2165,7 @@
         <v>2314</v>
       </c>
       <c r="C100" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="101" spans="2:3">
@@ -2172,7 +2173,7 @@
         <v>2317</v>
       </c>
       <c r="C101" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="102" spans="2:3">
@@ -2180,7 +2181,7 @@
         <v>2320</v>
       </c>
       <c r="C102" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="103" spans="2:3">
@@ -2188,7 +2189,7 @@
         <v>2323</v>
       </c>
       <c r="C103" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="104" spans="2:3">
@@ -2196,7 +2197,7 @@
         <v>2327</v>
       </c>
       <c r="C104" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="105" spans="2:3">
@@ -2204,7 +2205,7 @@
         <v>2329</v>
       </c>
       <c r="C105" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="106" spans="2:3">
@@ -2212,7 +2213,7 @@
         <v>2331</v>
       </c>
       <c r="C106" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="107" spans="2:3">
@@ -2220,7 +2221,7 @@
         <v>2334</v>
       </c>
       <c r="C107" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="108" spans="2:3">
@@ -2228,7 +2229,7 @@
         <v>2336</v>
       </c>
       <c r="C108" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="109" spans="2:3">
@@ -2236,7 +2237,7 @@
         <v>2338</v>
       </c>
       <c r="C109" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="110" spans="2:3">
@@ -2244,7 +2245,7 @@
         <v>2340</v>
       </c>
       <c r="C110" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="111" spans="2:3">
@@ -2252,7 +2253,7 @@
         <v>2342</v>
       </c>
       <c r="C111" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="112" spans="2:3">
@@ -2260,7 +2261,7 @@
         <v>2344</v>
       </c>
       <c r="C112" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="113" spans="2:4">
@@ -2268,7 +2269,7 @@
         <v>2356</v>
       </c>
       <c r="C113" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="114" spans="2:4">
@@ -2276,7 +2277,7 @@
         <v>2358</v>
       </c>
       <c r="C114" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="115" spans="2:4">
@@ -2284,7 +2285,7 @@
         <v>2360</v>
       </c>
       <c r="C115" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="116" spans="2:4">
@@ -2292,7 +2293,7 @@
         <v>2362</v>
       </c>
       <c r="C116" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="117" spans="2:4">
@@ -2300,7 +2301,7 @@
         <v>2364</v>
       </c>
       <c r="C117" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D117" s="1">
         <v>1</v>
@@ -2311,7 +2312,7 @@
         <v>2367</v>
       </c>
       <c r="C118" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D118" s="1">
         <v>1</v>
@@ -2322,7 +2323,7 @@
         <v>2370</v>
       </c>
       <c r="C119" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D119" s="1">
         <v>1</v>
@@ -2333,7 +2334,7 @@
         <v>2384</v>
       </c>
       <c r="C120" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="121" spans="2:4">
@@ -2341,7 +2342,7 @@
         <v>2387</v>
       </c>
       <c r="C121" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="122" spans="2:4">
@@ -2349,7 +2350,7 @@
         <v>2469</v>
       </c>
       <c r="C122" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="123" spans="2:4">
@@ -2357,7 +2358,7 @@
         <v>2472</v>
       </c>
       <c r="C123" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="124" spans="2:4">
@@ -2365,7 +2366,7 @@
         <v>2475</v>
       </c>
       <c r="C124" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="125" spans="2:4">
@@ -2373,7 +2374,7 @@
         <v>2478</v>
       </c>
       <c r="C125" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="126" spans="2:4">
@@ -2381,7 +2382,7 @@
         <v>2532</v>
       </c>
       <c r="C126" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="127" spans="2:4">
@@ -2389,7 +2390,7 @@
         <v>2536</v>
       </c>
       <c r="C127" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="128" spans="2:4">
@@ -2397,7 +2398,7 @@
         <v>2540</v>
       </c>
       <c r="C128" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="129" spans="2:4">
@@ -2405,7 +2406,7 @@
         <v>2542</v>
       </c>
       <c r="C129" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="130" spans="2:4">
@@ -2413,7 +2414,7 @@
         <v>2545</v>
       </c>
       <c r="C130" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="131" spans="2:4">
@@ -2421,7 +2422,7 @@
         <v>2547</v>
       </c>
       <c r="C131" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="132" spans="2:4">
@@ -2429,7 +2430,7 @@
         <v>2549</v>
       </c>
       <c r="C132" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="133" spans="2:4">
@@ -2437,7 +2438,7 @@
         <v>2551</v>
       </c>
       <c r="C133" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="134" spans="2:4">
@@ -2445,7 +2446,7 @@
         <v>2553</v>
       </c>
       <c r="C134" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="135" spans="2:4">
@@ -2453,7 +2454,7 @@
         <v>2556</v>
       </c>
       <c r="C135" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="136" spans="2:4">
@@ -2461,7 +2462,7 @@
         <v>2568</v>
       </c>
       <c r="C136" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="137" spans="2:4">
@@ -2469,7 +2470,7 @@
         <v>2573</v>
       </c>
       <c r="C137" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="138" spans="2:4">
@@ -2477,7 +2478,7 @@
         <v>2579</v>
       </c>
       <c r="C138" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="139" spans="2:4">
@@ -2485,7 +2486,7 @@
         <v>2582</v>
       </c>
       <c r="C139" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="140" spans="2:4">
@@ -2493,7 +2494,7 @@
         <v>2585</v>
       </c>
       <c r="C140" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="141" spans="2:4">
@@ -2501,7 +2502,7 @@
         <v>2586</v>
       </c>
       <c r="C141" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="142" spans="2:4">
@@ -2509,7 +2510,7 @@
         <v>2589</v>
       </c>
       <c r="C142" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D142" s="1">
         <v>1</v>
@@ -2520,7 +2521,7 @@
         <v>2593</v>
       </c>
       <c r="C143" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D143" s="1">
         <v>1</v>
@@ -2531,7 +2532,7 @@
         <v>2598</v>
       </c>
       <c r="C144" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D144" s="1">
         <v>1</v>
@@ -2542,7 +2543,7 @@
         <v>2603</v>
       </c>
       <c r="C145" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D145" s="1">
         <v>1</v>
@@ -2553,7 +2554,7 @@
         <v>2608</v>
       </c>
       <c r="C146" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D146" s="1">
         <v>1</v>
@@ -2564,7 +2565,7 @@
         <v>2614</v>
       </c>
       <c r="C147" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D147" s="1">
         <v>1</v>
@@ -2575,7 +2576,7 @@
         <v>2618</v>
       </c>
       <c r="C148" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D148" s="1">
         <v>1</v>
@@ -2586,7 +2587,7 @@
         <v>2621</v>
       </c>
       <c r="C149" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D149" s="1">
         <v>1</v>
@@ -2597,7 +2598,7 @@
         <v>2626</v>
       </c>
       <c r="C150" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D150" s="1">
         <v>1</v>
@@ -2608,7 +2609,7 @@
         <v>2631</v>
       </c>
       <c r="C151" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D151" s="1">
         <v>1</v>
@@ -2619,7 +2620,7 @@
         <v>2636</v>
       </c>
       <c r="C152" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="153" spans="2:4">
@@ -2627,7 +2628,7 @@
         <v>2640</v>
       </c>
       <c r="C153" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="154" spans="2:4">
@@ -2635,7 +2636,7 @@
         <v>2645</v>
       </c>
       <c r="C154" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D154" s="1">
         <v>1</v>
@@ -2646,7 +2647,7 @@
         <v>2648</v>
       </c>
       <c r="C155" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D155" s="1">
         <v>1</v>
@@ -2657,7 +2658,7 @@
         <v>2680</v>
       </c>
       <c r="C156" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="157" spans="2:4">
@@ -2665,7 +2666,7 @@
         <v>2698</v>
       </c>
       <c r="C157" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D157" s="1">
         <v>1</v>
@@ -2676,7 +2677,7 @@
         <v>2704</v>
       </c>
       <c r="C158" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D158" s="1">
         <v>1</v>
@@ -2687,7 +2688,7 @@
         <v>3278</v>
       </c>
       <c r="C159" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="160" spans="2:4">
@@ -2695,7 +2696,7 @@
         <v>3280</v>
       </c>
       <c r="C160" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="161" spans="2:4">
@@ -2703,7 +2704,7 @@
         <v>3628</v>
       </c>
       <c r="C161" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D161" s="1">
         <v>1</v>
@@ -2714,7 +2715,7 @@
         <v>3631</v>
       </c>
       <c r="C162" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="163" spans="2:4">
@@ -2722,7 +2723,7 @@
         <v>3633</v>
       </c>
       <c r="C163" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="164" spans="2:4">
@@ -2730,7 +2731,7 @@
         <v>4791</v>
       </c>
       <c r="C164" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="165" spans="2:4">
@@ -2738,7 +2739,7 @@
         <v>81</v>
       </c>
       <c r="C165" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="166" spans="2:4">
@@ -2746,7 +2747,7 @@
         <v>82</v>
       </c>
       <c r="C166" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="167" spans="2:4">
@@ -2754,7 +2755,7 @@
         <v>83</v>
       </c>
       <c r="C167" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="168" spans="2:4">
@@ -2762,7 +2763,7 @@
         <v>84</v>
       </c>
       <c r="C168" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="169" spans="2:4">
@@ -2770,7 +2771,7 @@
         <v>85</v>
       </c>
       <c r="C169" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="170" spans="2:4">
@@ -2778,7 +2779,7 @@
         <v>89</v>
       </c>
       <c r="C170" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="171" spans="2:4">
@@ -2786,7 +2787,7 @@
         <v>90</v>
       </c>
       <c r="C171" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="172" spans="2:4">
@@ -2794,7 +2795,7 @@
         <v>110</v>
       </c>
       <c r="C172" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="173" spans="2:4">
@@ -2802,7 +2803,7 @@
         <v>111</v>
       </c>
       <c r="C173" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="174" spans="2:4">
@@ -2810,7 +2811,7 @@
         <v>112</v>
       </c>
       <c r="C174" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="175" spans="2:4">
@@ -2818,7 +2819,7 @@
         <v>113</v>
       </c>
       <c r="C175" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="176" spans="2:4">
@@ -2826,7 +2827,7 @@
         <v>115</v>
       </c>
       <c r="C176" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="177" spans="2:4">
@@ -2834,7 +2835,7 @@
         <v>116</v>
       </c>
       <c r="C177" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="178" spans="2:4">
@@ -2842,7 +2843,7 @@
         <v>117</v>
       </c>
       <c r="C178" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="179" spans="2:4">
@@ -2850,7 +2851,7 @@
         <v>118</v>
       </c>
       <c r="C179" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="180" spans="2:4">
@@ -2858,7 +2859,7 @@
         <v>143</v>
       </c>
       <c r="C180" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="181" spans="2:4">
@@ -2866,7 +2867,7 @@
         <v>370</v>
       </c>
       <c r="C181" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="182" spans="2:4">
@@ -2874,7 +2875,7 @@
         <v>412</v>
       </c>
       <c r="C182" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="183" spans="2:4">
@@ -2882,7 +2883,7 @@
         <v>453</v>
       </c>
       <c r="C183" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="184" spans="2:4">
@@ -2890,7 +2891,7 @@
         <v>602</v>
       </c>
       <c r="C184" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="185" spans="2:4">
@@ -2898,7 +2899,7 @@
         <v>698</v>
       </c>
       <c r="C185" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="186" spans="2:4">
@@ -2906,7 +2907,7 @@
         <v>734</v>
       </c>
       <c r="C186" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="187" spans="2:4">
@@ -2914,7 +2915,7 @@
         <v>777</v>
       </c>
       <c r="C187" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="188" spans="2:4">
@@ -2922,7 +2923,7 @@
         <v>816</v>
       </c>
       <c r="C188" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="189" spans="2:4">
@@ -2930,7 +2931,7 @@
         <v>851</v>
       </c>
       <c r="C189" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="190" spans="2:4">
@@ -2938,7 +2939,7 @@
         <v>912</v>
       </c>
       <c r="C190" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D190" s="1">
         <v>1</v>
@@ -2949,7 +2950,7 @@
         <v>940</v>
       </c>
       <c r="C191" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D191" s="1">
         <v>1</v>
@@ -2960,7 +2961,7 @@
         <v>978</v>
       </c>
       <c r="C192" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D192" s="1">
         <v>1</v>
@@ -2971,7 +2972,7 @@
         <v>1267</v>
       </c>
       <c r="C193" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="194" spans="2:4">
@@ -2979,7 +2980,7 @@
         <v>1311</v>
       </c>
       <c r="C194" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D194" s="1">
         <v>1</v>
@@ -2990,7 +2991,7 @@
         <v>1399</v>
       </c>
       <c r="C195" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D195" s="1">
         <v>1</v>
@@ -3001,7 +3002,7 @@
         <v>1465</v>
       </c>
       <c r="C196" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="197" spans="2:4">
@@ -3009,7 +3010,7 @@
         <v>1687</v>
       </c>
       <c r="C197" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D197" s="1">
         <v>1</v>
@@ -3020,7 +3021,7 @@
         <v>2018</v>
       </c>
       <c r="C198" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="199" spans="2:4">
@@ -3028,7 +3029,7 @@
         <v>2057</v>
       </c>
       <c r="C199" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="200" spans="2:4">
@@ -3036,7 +3037,7 @@
         <v>2090</v>
       </c>
       <c r="C200" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D200" s="1">
         <v>1</v>
@@ -3047,7 +3048,7 @@
         <v>2444</v>
       </c>
       <c r="C201" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="202" spans="2:4">
@@ -3055,7 +3056,7 @@
         <v>2495</v>
       </c>
       <c r="C202" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="203" spans="2:4">
@@ -3063,7 +3064,7 @@
         <v>2656</v>
       </c>
       <c r="C203" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="204" spans="2:4">
@@ -3071,7 +3072,7 @@
         <v>2755</v>
       </c>
       <c r="C204" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="205" spans="2:4">
@@ -3079,7 +3080,7 @@
         <v>2926</v>
       </c>
       <c r="C205" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="206" spans="2:4">
@@ -3087,7 +3088,7 @@
         <v>2987</v>
       </c>
       <c r="C206" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="207" spans="2:4">
@@ -3095,7 +3096,7 @@
         <v>3038</v>
       </c>
       <c r="C207" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="208" spans="2:4">
@@ -3103,7 +3104,7 @@
         <v>3079</v>
       </c>
       <c r="C208" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="209" spans="2:3">
@@ -3111,7 +3112,7 @@
         <v>3094</v>
       </c>
       <c r="C209" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="210" spans="2:3">
@@ -3119,7 +3120,7 @@
         <v>3109</v>
       </c>
       <c r="C210" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="211" spans="2:3">
@@ -3127,7 +3128,7 @@
         <v>3120</v>
       </c>
       <c r="C211" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="212" spans="2:3">
@@ -3135,7 +3136,7 @@
         <v>3155</v>
       </c>
       <c r="C212" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="213" spans="2:3">
@@ -3143,7 +3144,7 @@
         <v>3238</v>
       </c>
       <c r="C213" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="214" spans="2:3">
@@ -3151,7 +3152,7 @@
         <v>3285</v>
       </c>
       <c r="C214" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="215" spans="2:3">
@@ -3159,7 +3160,7 @@
         <v>3286</v>
       </c>
       <c r="C215" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="216" spans="2:3">
@@ -3167,7 +3168,7 @@
         <v>3287</v>
       </c>
       <c r="C216" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="217" spans="2:3">
@@ -3175,7 +3176,7 @@
         <v>3288</v>
       </c>
       <c r="C217" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="218" spans="2:3">
@@ -3183,7 +3184,7 @@
         <v>3375</v>
       </c>
       <c r="C218" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="219" spans="2:3">
@@ -3191,7 +3192,7 @@
         <v>3647</v>
       </c>
       <c r="C219" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="220" spans="2:3">
@@ -3199,7 +3200,7 @@
         <v>3688</v>
       </c>
       <c r="C220" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="221" spans="2:3">
@@ -3207,7 +3208,7 @@
         <v>3726</v>
       </c>
       <c r="C221" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="222" spans="2:3">
@@ -3215,7 +3216,7 @@
         <v>3800</v>
       </c>
       <c r="C222" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="223" spans="2:3">
@@ -3223,7 +3224,7 @@
         <v>3830</v>
       </c>
       <c r="C223" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="224" spans="2:3">
@@ -3231,7 +3232,7 @@
         <v>3880</v>
       </c>
       <c r="C224" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="225" spans="2:4">
@@ -3239,7 +3240,7 @@
         <v>4039</v>
       </c>
       <c r="C225" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="226" spans="2:4">
@@ -3247,7 +3248,7 @@
         <v>4118</v>
       </c>
       <c r="C226" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="227" spans="2:4">
@@ -3255,7 +3256,7 @@
         <v>4106</v>
       </c>
       <c r="C227" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="228" spans="2:4">
@@ -3263,7 +3264,7 @@
         <v>4248</v>
       </c>
       <c r="C228" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="229" spans="2:4">
@@ -3271,7 +3272,7 @@
         <v>4262</v>
       </c>
       <c r="C229" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="230" spans="2:4">
@@ -3279,7 +3280,7 @@
         <v>4345</v>
       </c>
       <c r="C230" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="231" spans="2:4">
@@ -3287,7 +3288,7 @@
         <v>4389</v>
       </c>
       <c r="C231" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D231" s="1">
         <v>1</v>
@@ -3298,7 +3299,7 @@
         <v>4464</v>
       </c>
       <c r="C232" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="233" spans="2:4">
@@ -3306,7 +3307,7 @@
         <v>4714</v>
       </c>
       <c r="C233" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="234" spans="2:4">
@@ -3314,7 +3315,7 @@
         <v>4784</v>
       </c>
       <c r="C234" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="235" spans="2:4">
@@ -3322,7 +3323,7 @@
         <v>4795</v>
       </c>
       <c r="C235" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="236" spans="2:4">
@@ -3330,7 +3331,7 @@
         <v>4812</v>
       </c>
       <c r="C236" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="237" spans="2:4">
@@ -3338,7 +3339,7 @@
         <v>4824</v>
       </c>
       <c r="C237" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="238" spans="2:4">
@@ -3346,7 +3347,7 @@
         <v>4839</v>
       </c>
       <c r="C238" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added sample that normal array operations
</commit_message>
<xml_diff>
--- a/src/wrapped_functions_c++.xlsx
+++ b/src/wrapped_functions_c++.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">core.hpp!$B$1:$C$238</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -766,8 +766,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -823,13 +823,12 @@
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="7">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -837,12 +836,6 @@
           <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
@@ -872,16 +865,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="テーブル2" displayName="テーブル2" ref="B2:F3" totalsRowShown="0">
   <autoFilter ref="B2:F3"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="module" dataDxfId="7"/>
+    <tableColumn id="1" name="module" dataDxfId="6"/>
     <tableColumn id="2" name="Total"/>
-    <tableColumn id="3" name="Wrapped" dataDxfId="6">
+    <tableColumn id="3" name="Wrapped" dataDxfId="5">
       <calculatedColumnFormula>COUNTIF(テーブル1[Wrapped],1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Unwrapped" dataDxfId="5">
+    <tableColumn id="4" name="Unwrapped" dataDxfId="4">
       <calculatedColumnFormula>テーブル2[[#This Row],[Total]]-テーブル2[[#This Row],[Wrapped]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="%" dataDxfId="4">
-      <calculatedColumnFormula>テーブル2[Wrapped]/テーブル2[Total]</calculatedColumnFormula>
+    <tableColumn id="5" name="%" dataDxfId="3">
+      <calculatedColumnFormula>[Wrapped]/[Total]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -892,16 +885,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="テーブル1" displayName="テーブル1" ref="B1:D238" totalsRowShown="0">
   <autoFilter ref="B1:D238"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Line" dataDxfId="3"/>
+    <tableColumn id="1" name="Line" dataDxfId="1"/>
     <tableColumn id="2" name="Definition"/>
-    <tableColumn id="3" name="Wrapped" dataDxfId="2"/>
+    <tableColumn id="3" name="Wrapped" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office ​​テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -975,7 +968,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1010,7 +1002,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1186,14 +1177,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
@@ -1201,7 +1192,7 @@
     <col min="5" max="5" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:6">
       <c r="B2" t="s">
         <v>244</v>
       </c>
@@ -1218,7 +1209,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:6">
       <c r="B3" s="3" t="s">
         <v>166</v>
       </c>
@@ -1228,15 +1219,15 @@
       </c>
       <c r="D3">
         <f>COUNTIF(テーブル1[Wrapped],1)</f>
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E3">
         <f>テーブル2[[#This Row],[Total]]-テーブル2[[#This Row],[Wrapped]]</f>
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F3" s="2">
-        <f>テーブル2[Wrapped]/テーブル2[Total]</f>
-        <v>0.30379746835443039</v>
+        <f>[Wrapped]/[Total]</f>
+        <v>0.31645569620253167</v>
       </c>
     </row>
   </sheetData>
@@ -1250,22 +1241,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:D238"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E224" sqref="E224"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="2" max="2" width="7.625" style="1" customWidth="1"/>
     <col min="3" max="3" width="84" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:4">
       <c r="B1" s="1" t="s">
         <v>163</v>
       </c>
@@ -1276,7 +1267,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:4">
       <c r="B2" s="1">
         <v>123</v>
       </c>
@@ -1284,7 +1275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:4">
       <c r="B3" s="1">
         <v>124</v>
       </c>
@@ -1292,7 +1283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:4">
       <c r="B4" s="1">
         <v>127</v>
       </c>
@@ -1300,7 +1291,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:4">
       <c r="B5" s="1">
         <v>128</v>
       </c>
@@ -1308,7 +1299,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:4">
       <c r="B6" s="1">
         <v>182</v>
       </c>
@@ -1316,7 +1307,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:4">
       <c r="B7" s="1">
         <v>192</v>
       </c>
@@ -1324,7 +1315,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:4">
       <c r="B8" s="1">
         <v>209</v>
       </c>
@@ -1332,7 +1323,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:4">
       <c r="B9" s="1">
         <v>231</v>
       </c>
@@ -1340,7 +1331,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:4">
       <c r="B10" s="1">
         <v>233</v>
       </c>
@@ -1351,7 +1342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:4">
       <c r="B11" s="1">
         <v>234</v>
       </c>
@@ -1362,7 +1353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:4">
       <c r="B12" s="1">
         <v>235</v>
       </c>
@@ -1373,7 +1364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:4">
       <c r="B13" s="1">
         <v>237</v>
       </c>
@@ -1384,7 +1375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:4">
       <c r="B14" s="1">
         <v>247</v>
       </c>
@@ -1395,7 +1386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:4">
       <c r="B15" s="1">
         <v>261</v>
       </c>
@@ -1406,7 +1397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:4">
       <c r="B16" s="1">
         <v>271</v>
       </c>
@@ -1417,7 +1408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:4">
       <c r="B17" s="1">
         <v>292</v>
       </c>
@@ -1428,7 +1419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:4">
       <c r="B18" s="1">
         <v>295</v>
       </c>
@@ -1439,7 +1430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:4">
       <c r="B19" s="1">
         <v>307</v>
       </c>
@@ -1450,7 +1441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:4">
       <c r="B20" s="1">
         <v>315</v>
       </c>
@@ -1461,7 +1452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:4">
       <c r="B21" s="1">
         <v>358</v>
       </c>
@@ -1472,7 +1463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:4">
       <c r="B22" s="1">
         <v>365</v>
       </c>
@@ -1483,7 +1474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:4">
       <c r="B23" s="1">
         <v>969</v>
       </c>
@@ -1491,7 +1482,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:4">
       <c r="B24" s="1">
         <v>1453</v>
       </c>
@@ -1499,7 +1490,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:4">
       <c r="B25" s="1">
         <v>2120</v>
       </c>
@@ -1507,7 +1498,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:4">
       <c r="B26" s="1">
         <v>2121</v>
       </c>
@@ -1515,7 +1506,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:4">
       <c r="B27" s="1">
         <v>2122</v>
       </c>
@@ -1523,7 +1514,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:4">
       <c r="B28" s="1">
         <v>2125</v>
       </c>
@@ -1531,7 +1522,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:4">
       <c r="B29" s="1">
         <v>2128</v>
       </c>
@@ -1542,7 +1533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:4">
       <c r="B30" s="1">
         <v>2131</v>
       </c>
@@ -1553,7 +1544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:4">
       <c r="B31" s="1">
         <v>2133</v>
       </c>
@@ -1564,7 +1555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:4">
       <c r="B32" s="1">
         <v>2136</v>
       </c>
@@ -1575,7 +1566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:4">
       <c r="B33" s="1">
         <v>2139</v>
       </c>
@@ -1586,7 +1577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:4">
       <c r="B34" s="1">
         <v>2143</v>
       </c>
@@ -1597,7 +1588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:4">
       <c r="B35" s="1">
         <v>2147</v>
       </c>
@@ -1608,7 +1599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:4">
       <c r="B36" s="1">
         <v>2151</v>
       </c>
@@ -1619,7 +1610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:4">
       <c r="B37" s="1">
         <v>2155</v>
       </c>
@@ -1630,7 +1621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:4">
       <c r="B38" s="1">
         <v>2158</v>
       </c>
@@ -1641,7 +1632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:4">
       <c r="B39" s="1">
         <v>2162</v>
       </c>
@@ -1652,7 +1643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:4">
       <c r="B40" s="1">
         <v>2165</v>
       </c>
@@ -1663,7 +1654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="41" spans="2:4">
       <c r="B41" s="1">
         <v>2169</v>
       </c>
@@ -1674,7 +1665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:4">
       <c r="B42" s="1">
         <v>2171</v>
       </c>
@@ -1685,7 +1676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="43" spans="2:4">
       <c r="B43" s="1">
         <v>2173</v>
       </c>
@@ -1696,7 +1687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="44" spans="2:4">
       <c r="B44" s="1">
         <v>2176</v>
       </c>
@@ -1707,7 +1698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="45" spans="2:4">
       <c r="B45" s="1">
         <v>2178</v>
       </c>
@@ -1718,7 +1709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="46" spans="2:4">
       <c r="B46" s="1">
         <v>2181</v>
       </c>
@@ -1729,7 +1720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="47" spans="2:4">
       <c r="B47" s="1">
         <v>2183</v>
       </c>
@@ -1740,7 +1731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="48" spans="2:4">
       <c r="B48" s="1">
         <v>2187</v>
       </c>
@@ -1751,7 +1742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="49" spans="2:4">
       <c r="B49" s="1">
         <v>2194</v>
       </c>
@@ -1762,7 +1753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="50" spans="2:4">
       <c r="B50" s="1">
         <v>2198</v>
       </c>
@@ -1773,7 +1764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="51" spans="2:4">
       <c r="B51" s="1">
         <v>2201</v>
       </c>
@@ -1784,7 +1775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="52" spans="2:4">
       <c r="B52" s="1">
         <v>2205</v>
       </c>
@@ -1795,7 +1786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="53" spans="2:4">
       <c r="B53" s="1">
         <v>2208</v>
       </c>
@@ -1806,7 +1797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="54" spans="2:4">
       <c r="B54" s="1">
         <v>2209</v>
       </c>
@@ -1817,7 +1808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="55" spans="2:4">
       <c r="B55" s="1">
         <v>2212</v>
       </c>
@@ -1828,7 +1819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="56" spans="2:4">
       <c r="B56" s="1">
         <v>2215</v>
       </c>
@@ -1839,7 +1830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="57" spans="2:4">
       <c r="B57" s="1">
         <v>2216</v>
       </c>
@@ -1850,7 +1841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="58" spans="2:4">
       <c r="B58" s="1">
         <v>2219</v>
       </c>
@@ -1861,31 +1852,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="59" spans="2:4">
       <c r="B59" s="1">
         <v>2222</v>
       </c>
       <c r="C59" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="D59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4">
       <c r="B60" s="1">
         <v>2224</v>
       </c>
       <c r="C60" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="D60" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4">
       <c r="B61" s="1">
         <v>2226</v>
       </c>
       <c r="C61" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="D61" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4">
       <c r="B62" s="1">
         <v>2230</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="63" spans="2:4">
       <c r="B63" s="1">
         <v>2233</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="64" spans="2:4">
       <c r="B64" s="1">
         <v>2236</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="65" spans="2:4">
       <c r="B65" s="1">
         <v>2239</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="66" spans="2:4">
       <c r="B66" s="1">
         <v>2240</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="67" spans="2:4">
       <c r="B67" s="1">
         <v>2242</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="68" spans="2:4">
       <c r="B68" s="1">
         <v>2243</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="69" spans="2:4">
       <c r="B69" s="1">
         <v>2244</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="70" spans="2:4">
       <c r="B70" s="1">
         <v>2246</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="71" spans="2:4">
       <c r="B71" s="1">
         <v>2247</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="72" spans="2:4">
       <c r="B72" s="1">
         <v>2248</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="73" spans="2:4">
       <c r="B73" s="1">
         <v>2251</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="74" spans="2:4">
       <c r="B74" s="1">
         <v>2254</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="75" spans="2:4">
       <c r="B75" s="1">
         <v>2257</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="76" spans="2:4">
       <c r="B76" s="1">
         <v>2260</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="77" spans="2:4">
       <c r="B77" s="1">
         <v>2263</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="78" spans="2:4">
       <c r="B78" s="1">
         <v>2265</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="79" spans="2:4">
       <c r="B79" s="1">
         <v>2268</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="80" spans="2:4">
       <c r="B80" s="1">
         <v>2270</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="81" spans="2:3">
       <c r="B81" s="1">
         <v>2272</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="82" spans="2:3">
       <c r="B82" s="1">
         <v>2275</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="83" spans="2:3">
       <c r="B83" s="1">
         <v>2277</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="84" spans="2:3">
       <c r="B84" s="1">
         <v>2279</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="85" spans="2:3">
       <c r="B85" s="1">
         <v>2281</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="86" spans="2:3">
       <c r="B86" s="1">
         <v>2284</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="87" spans="2:3">
       <c r="B87" s="1">
         <v>2286</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="88" spans="2:3">
       <c r="B88" s="1">
         <v>2288</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="89" spans="2:3">
       <c r="B89" s="1">
         <v>2290</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="90" spans="2:3">
       <c r="B90" s="1">
         <v>2292</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="91" spans="2:3">
       <c r="B91" s="1">
         <v>2294</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="92" spans="2:3">
       <c r="B92" s="1">
         <v>2296</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="93" spans="2:3">
       <c r="B93" s="1">
         <v>2297</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="94" spans="2:3">
       <c r="B94" s="1">
         <v>2298</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="95" spans="2:3">
       <c r="B95" s="1">
         <v>2299</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="96" spans="2:3">
       <c r="B96" s="1">
         <v>2302</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="97" spans="2:3">
       <c r="B97" s="1">
         <v>2305</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="98" spans="2:3">
       <c r="B98" s="1">
         <v>2309</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="99" spans="2:3">
       <c r="B99" s="1">
         <v>2312</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="100" spans="2:3">
       <c r="B100" s="1">
         <v>2314</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="101" spans="2:3">
       <c r="B101" s="1">
         <v>2317</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="102" spans="2:3">
       <c r="B102" s="1">
         <v>2320</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="103" spans="2:3">
       <c r="B103" s="1">
         <v>2323</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="104" spans="2:3">
       <c r="B104" s="1">
         <v>2327</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="105" spans="2:3">
       <c r="B105" s="1">
         <v>2329</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="106" spans="2:3">
       <c r="B106" s="1">
         <v>2331</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="107" spans="2:3">
       <c r="B107" s="1">
         <v>2334</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="108" spans="2:3">
       <c r="B108" s="1">
         <v>2336</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="109" spans="2:3">
       <c r="B109" s="1">
         <v>2338</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="110" spans="2:3">
       <c r="B110" s="1">
         <v>2340</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="111" spans="2:3">
       <c r="B111" s="1">
         <v>2342</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="112" spans="2:3">
       <c r="B112" s="1">
         <v>2344</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="113" spans="2:4">
       <c r="B113" s="1">
         <v>2356</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="114" spans="2:4">
       <c r="B114" s="1">
         <v>2358</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="115" spans="2:4">
       <c r="B115" s="1">
         <v>2360</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="116" spans="2:4">
       <c r="B116" s="1">
         <v>2362</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="117" spans="2:4">
       <c r="B117" s="1">
         <v>2364</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="118" spans="2:4">
       <c r="B118" s="1">
         <v>2367</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="119" spans="2:4">
       <c r="B119" s="1">
         <v>2370</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="120" spans="2:4">
       <c r="B120" s="1">
         <v>2384</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="121" spans="2:4">
       <c r="B121" s="1">
         <v>2387</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="122" spans="2:4">
       <c r="B122" s="1">
         <v>2469</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="123" spans="2:4">
       <c r="B123" s="1">
         <v>2472</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="124" spans="2:4">
       <c r="B124" s="1">
         <v>2475</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="125" spans="2:4">
       <c r="B125" s="1">
         <v>2478</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="126" spans="2:4">
       <c r="B126" s="1">
         <v>2532</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="127" spans="2:4">
       <c r="B127" s="1">
         <v>2536</v>
       </c>
@@ -2434,7 +2434,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="128" spans="2:4">
       <c r="B128" s="1">
         <v>2540</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="129" spans="2:4">
       <c r="B129" s="1">
         <v>2542</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="130" spans="2:4">
       <c r="B130" s="1">
         <v>2545</v>
       </c>
@@ -2458,7 +2458,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="131" spans="2:4">
       <c r="B131" s="1">
         <v>2547</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="132" spans="2:4">
       <c r="B132" s="1">
         <v>2549</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="133" spans="2:4">
       <c r="B133" s="1">
         <v>2551</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="134" spans="2:4">
       <c r="B134" s="1">
         <v>2553</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="135" spans="2:4">
       <c r="B135" s="1">
         <v>2556</v>
       </c>
@@ -2498,7 +2498,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="136" spans="2:4">
       <c r="B136" s="1">
         <v>2568</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="137" spans="2:4">
       <c r="B137" s="1">
         <v>2573</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="138" spans="2:4">
       <c r="B138" s="1">
         <v>2579</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="139" spans="2:4">
       <c r="B139" s="1">
         <v>2582</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="140" spans="2:4">
       <c r="B140" s="1">
         <v>2585</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="141" spans="2:4">
       <c r="B141" s="1">
         <v>2586</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="142" spans="2:4">
       <c r="B142" s="1">
         <v>2589</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="143" spans="2:4">
       <c r="B143" s="1">
         <v>2593</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="144" spans="2:4">
       <c r="B144" s="1">
         <v>2598</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="145" spans="2:4">
       <c r="B145" s="1">
         <v>2603</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="146" spans="2:4">
       <c r="B146" s="1">
         <v>2608</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="147" spans="2:4">
       <c r="B147" s="1">
         <v>2614</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="148" spans="2:4">
       <c r="B148" s="1">
         <v>2618</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="149" spans="2:4">
       <c r="B149" s="1">
         <v>2621</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="150" spans="2:4">
       <c r="B150" s="1">
         <v>2626</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="151" spans="2:4">
       <c r="B151" s="1">
         <v>2631</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="152" spans="2:4">
       <c r="B152" s="1">
         <v>2636</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="153" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="153" spans="2:4">
       <c r="B153" s="1">
         <v>2640</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="154" spans="2:4">
       <c r="B154" s="1">
         <v>2645</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="155" spans="2:4">
       <c r="B155" s="1">
         <v>2648</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="156" spans="2:4">
       <c r="B156" s="1">
         <v>2680</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="157" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="157" spans="2:4">
       <c r="B157" s="1">
         <v>2698</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="158" spans="2:4">
       <c r="B158" s="1">
         <v>2704</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="159" spans="2:4">
       <c r="B159" s="1">
         <v>3278</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="160" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="160" spans="2:4">
       <c r="B160" s="1">
         <v>3280</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="161" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="161" spans="2:3">
       <c r="B161" s="1">
         <v>3628</v>
       </c>
@@ -2748,7 +2748,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="162" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="162" spans="2:3">
       <c r="B162" s="1">
         <v>3631</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="163" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="163" spans="2:3">
       <c r="B163" s="1">
         <v>3633</v>
       </c>
@@ -2764,7 +2764,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="164" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="164" spans="2:3">
       <c r="B164" s="1">
         <v>4791</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="165" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="165" spans="2:3">
       <c r="B165" s="1">
         <v>81</v>
       </c>
@@ -2780,7 +2780,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="166" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="166" spans="2:3">
       <c r="B166" s="1">
         <v>82</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="167" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="167" spans="2:3">
       <c r="B167" s="1">
         <v>83</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="168" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="168" spans="2:3">
       <c r="B168" s="1">
         <v>84</v>
       </c>
@@ -2804,7 +2804,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="169" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="169" spans="2:3">
       <c r="B169" s="1">
         <v>85</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="170" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="170" spans="2:3">
       <c r="B170" s="1">
         <v>89</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="171" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="171" spans="2:3">
       <c r="B171" s="1">
         <v>90</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="172" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="172" spans="2:3">
       <c r="B172" s="1">
         <v>110</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="173" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="173" spans="2:3">
       <c r="B173" s="1">
         <v>111</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="174" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="174" spans="2:3">
       <c r="B174" s="1">
         <v>112</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="175" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="175" spans="2:3">
       <c r="B175" s="1">
         <v>113</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="176" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="176" spans="2:3">
       <c r="B176" s="1">
         <v>115</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="177" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="177" spans="2:4">
       <c r="B177" s="1">
         <v>116</v>
       </c>
@@ -2876,7 +2876,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="178" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="178" spans="2:4">
       <c r="B178" s="1">
         <v>117</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="179" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="179" spans="2:4">
       <c r="B179" s="1">
         <v>118</v>
       </c>
@@ -2892,7 +2892,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="180" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="180" spans="2:4">
       <c r="B180" s="1">
         <v>143</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="181" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="181" spans="2:4">
       <c r="B181" s="1">
         <v>370</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="182" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="182" spans="2:4">
       <c r="B182" s="1">
         <v>412</v>
       </c>
@@ -2916,7 +2916,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="183" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="183" spans="2:4">
       <c r="B183" s="1">
         <v>453</v>
       </c>
@@ -2924,7 +2924,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="184" spans="2:4">
       <c r="B184" s="1">
         <v>602</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="185" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="185" spans="2:4">
       <c r="B185" s="1">
         <v>698</v>
       </c>
@@ -2940,7 +2940,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="186" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="186" spans="2:4">
       <c r="B186" s="1">
         <v>734</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="187" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="187" spans="2:4">
       <c r="B187" s="1">
         <v>777</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="188" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="188" spans="2:4">
       <c r="B188" s="1">
         <v>816</v>
       </c>
@@ -2964,7 +2964,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="189" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="189" spans="2:4">
       <c r="B189" s="1">
         <v>851</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="190" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="190" spans="2:4">
       <c r="B190" s="1">
         <v>912</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="191" spans="2:4">
       <c r="B191" s="1">
         <v>940</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="192" spans="2:4">
       <c r="B192" s="1">
         <v>978</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="193" spans="2:4">
       <c r="B193" s="1">
         <v>1267</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="194" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="194" spans="2:4">
       <c r="B194" s="1">
         <v>1311</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="195" spans="2:4">
       <c r="B195" s="1">
         <v>1399</v>
       </c>
@@ -3035,7 +3035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="196" spans="2:4">
       <c r="B196" s="1">
         <v>1465</v>
       </c>
@@ -3043,7 +3043,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="197" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="197" spans="2:4">
       <c r="B197" s="1">
         <v>1687</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="198" spans="2:4">
       <c r="B198" s="1">
         <v>2018</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="199" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="199" spans="2:4">
       <c r="B199" s="1">
         <v>2057</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="200" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="200" spans="2:4">
       <c r="B200" s="1">
         <v>2090</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="201" spans="2:4">
       <c r="B201" s="1">
         <v>2444</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="202" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="202" spans="2:4">
       <c r="B202" s="1">
         <v>2495</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="203" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="203" spans="2:4">
       <c r="B203" s="1">
         <v>2656</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="204" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="204" spans="2:4">
       <c r="B204" s="1">
         <v>2755</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="205" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="205" spans="2:4">
       <c r="B205" s="1">
         <v>2926</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="206" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="206" spans="2:4">
       <c r="B206" s="1">
         <v>2987</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="207" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="207" spans="2:4">
       <c r="B207" s="1">
         <v>3038</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="208" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="208" spans="2:4">
       <c r="B208" s="1">
         <v>3079</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="209" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="209" spans="2:3">
       <c r="B209" s="1">
         <v>3094</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="210" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="210" spans="2:3">
       <c r="B210" s="1">
         <v>3109</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="211" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="211" spans="2:3">
       <c r="B211" s="1">
         <v>3120</v>
       </c>
@@ -3169,7 +3169,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="212" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="212" spans="2:3">
       <c r="B212" s="1">
         <v>3155</v>
       </c>
@@ -3177,7 +3177,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="213" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="213" spans="2:3">
       <c r="B213" s="1">
         <v>3238</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="214" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="214" spans="2:3">
       <c r="B214" s="1">
         <v>3285</v>
       </c>
@@ -3193,7 +3193,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="215" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="215" spans="2:3">
       <c r="B215" s="1">
         <v>3286</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="216" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="216" spans="2:3">
       <c r="B216" s="1">
         <v>3287</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="217" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="217" spans="2:3">
       <c r="B217" s="1">
         <v>3288</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="218" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="218" spans="2:3">
       <c r="B218" s="1">
         <v>3375</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="219" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="219" spans="2:3">
       <c r="B219" s="1">
         <v>3647</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="220" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="220" spans="2:3">
       <c r="B220" s="1">
         <v>3688</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="221" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="221" spans="2:3">
       <c r="B221" s="1">
         <v>3726</v>
       </c>
@@ -3249,7 +3249,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="222" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="222" spans="2:3">
       <c r="B222" s="1">
         <v>3800</v>
       </c>
@@ -3257,7 +3257,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="223" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="223" spans="2:3">
       <c r="B223" s="1">
         <v>3830</v>
       </c>
@@ -3265,7 +3265,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="224" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="224" spans="2:3">
       <c r="B224" s="1">
         <v>3880</v>
       </c>
@@ -3273,7 +3273,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="225" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="225" spans="2:4">
       <c r="B225" s="1">
         <v>4039</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="226" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="226" spans="2:4">
       <c r="B226" s="1">
         <v>4118</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="227" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="227" spans="2:4">
       <c r="B227" s="1">
         <v>4106</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="228" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="228" spans="2:4">
       <c r="B228" s="1">
         <v>4248</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="229" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="229" spans="2:4">
       <c r="B229" s="1">
         <v>4262</v>
       </c>
@@ -3313,7 +3313,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="230" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="230" spans="2:4">
       <c r="B230" s="1">
         <v>4345</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="231" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="231" spans="2:4">
       <c r="B231" s="1">
         <v>4389</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="232" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="232" spans="2:4">
       <c r="B232" s="1">
         <v>4464</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="233" spans="2:4">
       <c r="B233" s="1">
         <v>4714</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="234" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="234" spans="2:4">
       <c r="B234" s="1">
         <v>4784</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="235" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="235" spans="2:4">
       <c r="B235" s="1">
         <v>4795</v>
       </c>
@@ -3364,7 +3364,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="236" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="236" spans="2:4">
       <c r="B236" s="1">
         <v>4812</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="237" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="237" spans="2:4">
       <c r="B237" s="1">
         <v>4824</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="238" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="238" spans="2:4">
       <c r="B238" s="1">
         <v>4839</v>
       </c>
@@ -3391,7 +3391,7 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="B2:D238">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added SVD methods and class
</commit_message>
<xml_diff>
--- a/src/wrapped_functions_c++.xlsx
+++ b/src/wrapped_functions_c++.xlsx
@@ -1644,15 +1644,15 @@
       </c>
       <c r="D3">
         <f>COUNTIF(テーブル1[Wrapped],1)</f>
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E3">
         <f>テーブル2[[#This Row],[Total]]-テーブル2[[#This Row],[Wrapped]]</f>
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F3" s="2">
         <f>テーブル2[Wrapped]/テーブル2[Total]</f>
-        <v>0.56118143459915615</v>
+        <v>0.57383966244725737</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.15">
@@ -1691,8 +1691,8 @@
   <dimension ref="B1:D238"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F204" sqref="F204"/>
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C132" sqref="C132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3042,6 +3042,9 @@
       <c r="C126" t="s">
         <v>124</v>
       </c>
+      <c r="D126" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="127" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B127" s="1">
@@ -3050,6 +3053,9 @@
       <c r="C127" t="s">
         <v>125</v>
       </c>
+      <c r="D127" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="128" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B128" s="1">
@@ -3715,6 +3721,9 @@
       </c>
       <c r="C202" t="s">
         <v>206</v>
+      </c>
+      <c r="D202" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="203" spans="2:4" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
updated wrapped func list
</commit_message>
<xml_diff>
--- a/src/wrapped_functions_c++.xlsx
+++ b/src/wrapped_functions_c++.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="4" r:id="rId1"/>
@@ -13,14 +13,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">core.hpp!$B$1:$C$238</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">imgproc.hpp!$B$1:$C$131</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">imgproc.hpp!$B$1:$C$130</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="372">
   <si>
     <t>string fromUtf16(const WString&amp; str);</t>
   </si>
@@ -1011,9 +1011,6 @@
   </si>
   <si>
     <t>void undistortPoints( InputArray src, OutputArray dst,</t>
-  </si>
-  <si>
-    <t>template&lt;&gt; void Ptr&lt;CvHistogram&gt;::delete_obj();</t>
   </si>
   <si>
     <t>void calcHist( const Mat* images, int nimages,</t>
@@ -1222,10 +1219,11 @@
   </cellStyles>
   <dxfs count="10">
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1241,11 +1239,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
@@ -1295,21 +1292,21 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="テーブル1" displayName="テーブル1" ref="B1:D238" totalsRowShown="0">
   <autoFilter ref="B1:D238"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Line" dataDxfId="4"/>
+    <tableColumn id="1" name="Line" dataDxfId="5"/>
     <tableColumn id="2" name="Definition"/>
-    <tableColumn id="3" name="Wrapped" dataDxfId="3"/>
+    <tableColumn id="3" name="Wrapped" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="テーブル14" displayName="テーブル14" ref="B1:D131" totalsRowShown="0">
-  <autoFilter ref="B1:D131"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="テーブル14" displayName="テーブル14" ref="B1:D130" totalsRowShown="0">
+  <autoFilter ref="B1:D130"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Line" dataDxfId="1"/>
+    <tableColumn id="1" name="Line" dataDxfId="3"/>
     <tableColumn id="2" name="Definition"/>
-    <tableColumn id="3" name="Wrapped" dataDxfId="0"/>
+    <tableColumn id="3" name="Wrapped" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1631,7 +1628,7 @@
         <v>168</v>
       </c>
       <c r="F2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.15">
@@ -1657,23 +1654,23 @@
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B4" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C4">
         <f>ROWS(テーブル14[Wrapped])</f>
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D4" s="5">
         <f>COUNTIF(テーブル14[Wrapped],1)</f>
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E4" s="5">
         <f>テーブル2[[#This Row],[Total]]-テーブル2[[#This Row],[Wrapped]]</f>
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F4" s="2">
         <f>テーブル2[Wrapped]/テーブル2[Total]</f>
-        <v>0.3923076923076923</v>
+        <v>0.4573643410852713</v>
       </c>
     </row>
   </sheetData>
@@ -1690,7 +1687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D238"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D156" sqref="D156"/>
     </sheetView>
@@ -4068,7 +4065,7 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="B2:D238">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4082,11 +4079,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D131"/>
+  <dimension ref="B1:D130"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C138" sqref="C138"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4872,6 +4869,9 @@
       <c r="C78" t="s">
         <v>320</v>
       </c>
+      <c r="D78" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B79" s="1">
@@ -4880,6 +4880,9 @@
       <c r="C79" t="s">
         <v>321</v>
       </c>
+      <c r="D79" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="80" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B80" s="1">
@@ -4889,129 +4892,147 @@
         <v>322</v>
       </c>
     </row>
-    <row r="81" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B81" s="1">
         <v>679</v>
       </c>
       <c r="C81" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="82" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="D81" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B82" s="1">
         <v>685</v>
       </c>
       <c r="C82" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="83" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="D82" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B83" s="1">
         <v>696</v>
       </c>
       <c r="C83" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="84" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="D83" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B84" s="1">
         <v>702</v>
       </c>
       <c r="C84" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="85" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="D84" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B85" s="1">
         <v>706</v>
       </c>
       <c r="C85" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="86" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="D85" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B86" s="1">
-        <v>710</v>
+        <v>713</v>
       </c>
       <c r="C86" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="87" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="D86" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B87" s="1">
-        <v>713</v>
+        <v>719</v>
       </c>
       <c r="C87" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="88" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B88" s="1">
-        <v>719</v>
+        <v>725</v>
       </c>
       <c r="C88" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="89" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B89" s="1">
-        <v>725</v>
+        <v>733</v>
       </c>
       <c r="C89" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="90" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B90" s="1">
-        <v>733</v>
+        <v>739</v>
       </c>
       <c r="C90" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="91" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B91" s="1">
-        <v>739</v>
+        <v>744</v>
       </c>
       <c r="C91" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="92" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B92" s="1">
-        <v>744</v>
+        <v>749</v>
       </c>
       <c r="C92" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="93" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B93" s="1">
-        <v>749</v>
+        <v>753</v>
       </c>
       <c r="C93" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="94" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B94" s="1">
-        <v>753</v>
+        <v>758</v>
       </c>
       <c r="C94" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="95" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B95" s="1">
-        <v>758</v>
+        <v>761</v>
       </c>
       <c r="C95" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="96" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B96" s="1">
-        <v>761</v>
+        <v>764</v>
       </c>
       <c r="C96" t="s">
         <v>336</v>
@@ -5019,7 +5040,7 @@
     </row>
     <row r="97" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B97" s="1">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="C97" t="s">
         <v>337</v>
@@ -5027,7 +5048,7 @@
     </row>
     <row r="98" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B98" s="1">
-        <v>766</v>
+        <v>779</v>
       </c>
       <c r="C98" t="s">
         <v>338</v>
@@ -5035,7 +5056,7 @@
     </row>
     <row r="99" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B99" s="1">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="C99" t="s">
         <v>339</v>
@@ -5043,7 +5064,7 @@
     </row>
     <row r="100" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B100" s="1">
-        <v>781</v>
+        <v>786</v>
       </c>
       <c r="C100" t="s">
         <v>340</v>
@@ -5051,7 +5072,7 @@
     </row>
     <row r="101" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B101" s="1">
-        <v>786</v>
+        <v>789</v>
       </c>
       <c r="C101" t="s">
         <v>341</v>
@@ -5059,7 +5080,7 @@
     </row>
     <row r="102" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B102" s="1">
-        <v>789</v>
+        <v>812</v>
       </c>
       <c r="C102" t="s">
         <v>342</v>
@@ -5067,7 +5088,7 @@
     </row>
     <row r="103" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B103" s="1">
-        <v>812</v>
+        <v>823</v>
       </c>
       <c r="C103" t="s">
         <v>343</v>
@@ -5075,7 +5096,7 @@
     </row>
     <row r="104" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B104" s="1">
-        <v>823</v>
+        <v>828</v>
       </c>
       <c r="C104" t="s">
         <v>344</v>
@@ -5083,7 +5104,7 @@
     </row>
     <row r="105" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B105" s="1">
-        <v>828</v>
+        <v>834</v>
       </c>
       <c r="C105" t="s">
         <v>345</v>
@@ -5091,7 +5112,7 @@
     </row>
     <row r="106" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B106" s="1">
-        <v>834</v>
+        <v>840</v>
       </c>
       <c r="C106" t="s">
         <v>346</v>
@@ -5099,7 +5120,7 @@
     </row>
     <row r="107" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B107" s="1">
-        <v>840</v>
+        <v>1091</v>
       </c>
       <c r="C107" t="s">
         <v>347</v>
@@ -5107,7 +5128,7 @@
     </row>
     <row r="108" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B108" s="1">
-        <v>1091</v>
+        <v>1094</v>
       </c>
       <c r="C108" t="s">
         <v>348</v>
@@ -5115,7 +5136,7 @@
     </row>
     <row r="109" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B109" s="1">
-        <v>1094</v>
+        <v>1116</v>
       </c>
       <c r="C109" t="s">
         <v>349</v>
@@ -5123,15 +5144,15 @@
     </row>
     <row r="110" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B110" s="1">
-        <v>1116</v>
+        <v>1119</v>
       </c>
       <c r="C110" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="111" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B111" s="1">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="C111" t="s">
         <v>351</v>
@@ -5139,7 +5160,7 @@
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B112" s="1">
-        <v>1120</v>
+        <v>1126</v>
       </c>
       <c r="C112" t="s">
         <v>352</v>
@@ -5147,7 +5168,7 @@
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B113" s="1">
-        <v>1126</v>
+        <v>1149</v>
       </c>
       <c r="C113" t="s">
         <v>353</v>
@@ -5155,15 +5176,15 @@
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B114" s="1">
-        <v>1149</v>
+        <v>1154</v>
       </c>
       <c r="C114" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B115" s="1">
-        <v>1154</v>
+        <v>1158</v>
       </c>
       <c r="C115" t="s">
         <v>354</v>
@@ -5171,7 +5192,7 @@
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B116" s="1">
-        <v>1158</v>
+        <v>1165</v>
       </c>
       <c r="C116" t="s">
         <v>355</v>
@@ -5179,7 +5200,7 @@
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B117" s="1">
-        <v>1165</v>
+        <v>1170</v>
       </c>
       <c r="C117" t="s">
         <v>356</v>
@@ -5187,7 +5208,7 @@
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B118" s="1">
-        <v>1170</v>
+        <v>1172</v>
       </c>
       <c r="C118" t="s">
         <v>357</v>
@@ -5195,7 +5216,7 @@
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B119" s="1">
-        <v>1172</v>
+        <v>1174</v>
       </c>
       <c r="C119" t="s">
         <v>358</v>
@@ -5203,7 +5224,7 @@
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B120" s="1">
-        <v>1174</v>
+        <v>1176</v>
       </c>
       <c r="C120" t="s">
         <v>359</v>
@@ -5211,7 +5232,7 @@
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B121" s="1">
-        <v>1176</v>
+        <v>1178</v>
       </c>
       <c r="C121" t="s">
         <v>360</v>
@@ -5219,7 +5240,7 @@
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B122" s="1">
-        <v>1178</v>
+        <v>1181</v>
       </c>
       <c r="C122" t="s">
         <v>361</v>
@@ -5227,7 +5248,7 @@
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B123" s="1">
-        <v>1181</v>
+        <v>1184</v>
       </c>
       <c r="C123" t="s">
         <v>362</v>
@@ -5235,7 +5256,7 @@
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B124" s="1">
-        <v>1184</v>
+        <v>1187</v>
       </c>
       <c r="C124" t="s">
         <v>363</v>
@@ -5243,7 +5264,7 @@
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B125" s="1">
-        <v>1187</v>
+        <v>1190</v>
       </c>
       <c r="C125" t="s">
         <v>364</v>
@@ -5251,7 +5272,7 @@
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B126" s="1">
-        <v>1190</v>
+        <v>1193</v>
       </c>
       <c r="C126" t="s">
         <v>365</v>
@@ -5259,7 +5280,7 @@
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B127" s="1">
-        <v>1193</v>
+        <v>1197</v>
       </c>
       <c r="C127" t="s">
         <v>366</v>
@@ -5267,7 +5288,7 @@
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B128" s="1">
-        <v>1197</v>
+        <v>1200</v>
       </c>
       <c r="C128" t="s">
         <v>367</v>
@@ -5275,7 +5296,7 @@
     </row>
     <row r="129" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B129" s="1">
-        <v>1200</v>
+        <v>1203</v>
       </c>
       <c r="C129" t="s">
         <v>368</v>
@@ -5283,27 +5304,19 @@
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B130" s="1">
-        <v>1203</v>
+        <v>1206</v>
       </c>
       <c r="C130" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B131" s="1">
-        <v>1206</v>
-      </c>
-      <c r="C131" t="s">
-        <v>370</v>
-      </c>
-      <c r="D131" s="1">
+      <c r="D130" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="B2:D131">
-    <cfRule type="expression" dxfId="2" priority="1">
+  <conditionalFormatting sqref="B2:D130">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added contour methods in imgproc
</commit_message>
<xml_diff>
--- a/src/wrapped_functions_c++.xlsx
+++ b/src/wrapped_functions_c++.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
@@ -13,14 +13,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">core.hpp!$B$1:$C$238</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">imgproc.hpp!$B$1:$C$128</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">imgproc.hpp!$B$1:$C$127</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="369">
   <si>
     <t>string fromUtf16(const WString&amp; str);</t>
   </si>
@@ -1074,9 +1074,6 @@
   </si>
   <si>
     <t>void HuMoments( const Moments&amp; moments, double hu[7] );</t>
-  </si>
-  <si>
-    <t>void HuMoments( const Moments&amp; m, CV_OUT OutputArray hu );</t>
   </si>
   <si>
     <t>void matchTemplate( InputArray image, InputArray templ,</t>
@@ -1144,8 +1141,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1213,10 +1210,11 @@
   </cellStyles>
   <dxfs count="10">
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1226,17 +1224,16 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
@@ -1275,7 +1272,7 @@
       <calculatedColumnFormula>テーブル2[[#This Row],[Total]]-テーブル2[[#This Row],[Wrapped]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Progress" dataDxfId="6">
-      <calculatedColumnFormula>[Wrapped]/[Total]</calculatedColumnFormula>
+      <calculatedColumnFormula>テーブル2[Wrapped]/テーブル2[Total]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1286,28 +1283,28 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="テーブル1" displayName="テーブル1" ref="B1:D238" totalsRowShown="0">
   <autoFilter ref="B1:D238"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Line" dataDxfId="4"/>
+    <tableColumn id="1" name="Line" dataDxfId="5"/>
     <tableColumn id="2" name="Definition"/>
-    <tableColumn id="3" name="Wrapped" dataDxfId="3"/>
+    <tableColumn id="3" name="Wrapped" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="テーブル14" displayName="テーブル14" ref="B1:D128" totalsRowShown="0">
-  <autoFilter ref="B1:D128"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="テーブル14" displayName="テーブル14" ref="B1:D127" totalsRowShown="0">
+  <autoFilter ref="B1:D127"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Line" dataDxfId="1"/>
+    <tableColumn id="1" name="Line" dataDxfId="3"/>
     <tableColumn id="2" name="Definition"/>
-    <tableColumn id="3" name="Wrapped" dataDxfId="0"/>
+    <tableColumn id="3" name="Wrapped" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office ​​テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1381,6 +1378,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1415,6 +1413,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1590,14 +1589,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
@@ -1606,7 +1605,7 @@
     <col min="6" max="6" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
         <v>243</v>
       </c>
@@ -1620,10 +1619,10 @@
         <v>168</v>
       </c>
       <c r="F2" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
         <v>166</v>
       </c>
@@ -1640,29 +1639,29 @@
         <v>85</v>
       </c>
       <c r="F3" s="2">
-        <f>[Wrapped]/[Total]</f>
+        <f>テーブル2[Wrapped]/テーブル2[Total]</f>
         <v>0.64135021097046419</v>
       </c>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B4" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C4">
         <f>ROWS(テーブル14[Wrapped])</f>
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D4" s="5">
         <f>COUNTIF(テーブル14[Wrapped],1)</f>
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="E4" s="5">
         <f>テーブル2[[#This Row],[Total]]-テーブル2[[#This Row],[Wrapped]]</f>
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="F4" s="2">
-        <f>[Wrapped]/[Total]</f>
-        <v>0.59055118110236215</v>
+        <f>テーブル2[Wrapped]/テーブル2[Total]</f>
+        <v>0.76190476190476186</v>
       </c>
     </row>
   </sheetData>
@@ -1676,7 +1675,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D238"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1684,14 +1683,14 @@
       <selection pane="bottomLeft" activeCell="D156" sqref="D156"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="7.625" style="1" customWidth="1"/>
     <col min="3" max="3" width="84" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
         <v>163</v>
       </c>
@@ -1702,7 +1701,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B2" s="1">
         <v>123</v>
       </c>
@@ -1710,7 +1709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B3" s="1">
         <v>124</v>
       </c>
@@ -1718,7 +1717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B4" s="1">
         <v>127</v>
       </c>
@@ -1726,7 +1725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B5" s="1">
         <v>128</v>
       </c>
@@ -1734,7 +1733,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B6" s="1">
         <v>182</v>
       </c>
@@ -1742,7 +1741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B7" s="1">
         <v>192</v>
       </c>
@@ -1750,7 +1749,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B8" s="1">
         <v>209</v>
       </c>
@@ -1758,7 +1757,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B9" s="1">
         <v>231</v>
       </c>
@@ -1766,7 +1765,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B10" s="1">
         <v>233</v>
       </c>
@@ -1777,7 +1776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B11" s="1">
         <v>234</v>
       </c>
@@ -1788,7 +1787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B12" s="1">
         <v>235</v>
       </c>
@@ -1799,7 +1798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B13" s="1">
         <v>237</v>
       </c>
@@ -1810,7 +1809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:4">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B14" s="1">
         <v>247</v>
       </c>
@@ -1821,7 +1820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:4">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B15" s="1">
         <v>261</v>
       </c>
@@ -1832,7 +1831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:4">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B16" s="1">
         <v>271</v>
       </c>
@@ -1843,7 +1842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B17" s="1">
         <v>292</v>
       </c>
@@ -1854,7 +1853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B18" s="1">
         <v>295</v>
       </c>
@@ -1865,7 +1864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B19" s="1">
         <v>307</v>
       </c>
@@ -1876,7 +1875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B20" s="1">
         <v>315</v>
       </c>
@@ -1887,7 +1886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B21" s="1">
         <v>358</v>
       </c>
@@ -1898,7 +1897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B22" s="1">
         <v>365</v>
       </c>
@@ -1909,7 +1908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B23" s="1">
         <v>969</v>
       </c>
@@ -1917,7 +1916,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B24" s="1">
         <v>1453</v>
       </c>
@@ -1925,7 +1924,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="2:4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B25" s="1">
         <v>2120</v>
       </c>
@@ -1933,7 +1932,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="2:4">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B26" s="1">
         <v>2121</v>
       </c>
@@ -1941,7 +1940,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="2:4">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B27" s="1">
         <v>2122</v>
       </c>
@@ -1949,7 +1948,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="2:4">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B28" s="1">
         <v>2125</v>
       </c>
@@ -1957,7 +1956,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="2:4">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B29" s="1">
         <v>2128</v>
       </c>
@@ -1968,7 +1967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:4">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B30" s="1">
         <v>2131</v>
       </c>
@@ -1979,7 +1978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:4">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B31" s="1">
         <v>2133</v>
       </c>
@@ -1990,7 +1989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:4">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B32" s="1">
         <v>2136</v>
       </c>
@@ -2001,7 +2000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:4">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B33" s="1">
         <v>2139</v>
       </c>
@@ -2012,7 +2011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:4">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B34" s="1">
         <v>2143</v>
       </c>
@@ -2023,7 +2022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:4">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B35" s="1">
         <v>2147</v>
       </c>
@@ -2034,7 +2033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:4">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B36" s="1">
         <v>2151</v>
       </c>
@@ -2045,7 +2044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:4">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B37" s="1">
         <v>2155</v>
       </c>
@@ -2056,7 +2055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:4">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B38" s="1">
         <v>2158</v>
       </c>
@@ -2067,7 +2066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:4">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B39" s="1">
         <v>2162</v>
       </c>
@@ -2078,7 +2077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:4">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B40" s="1">
         <v>2165</v>
       </c>
@@ -2089,7 +2088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:4">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B41" s="1">
         <v>2169</v>
       </c>
@@ -2100,7 +2099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:4">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B42" s="1">
         <v>2171</v>
       </c>
@@ -2111,7 +2110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:4">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B43" s="1">
         <v>2173</v>
       </c>
@@ -2122,7 +2121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:4">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B44" s="1">
         <v>2176</v>
       </c>
@@ -2133,7 +2132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:4">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B45" s="1">
         <v>2178</v>
       </c>
@@ -2144,7 +2143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:4">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B46" s="1">
         <v>2181</v>
       </c>
@@ -2155,7 +2154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:4">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B47" s="1">
         <v>2183</v>
       </c>
@@ -2166,7 +2165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:4">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B48" s="1">
         <v>2187</v>
       </c>
@@ -2177,7 +2176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:4">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B49" s="1">
         <v>2194</v>
       </c>
@@ -2188,7 +2187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:4">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B50" s="1">
         <v>2198</v>
       </c>
@@ -2199,7 +2198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:4">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B51" s="1">
         <v>2201</v>
       </c>
@@ -2210,7 +2209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:4">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B52" s="1">
         <v>2205</v>
       </c>
@@ -2221,7 +2220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:4">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B53" s="1">
         <v>2208</v>
       </c>
@@ -2232,7 +2231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:4">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B54" s="1">
         <v>2209</v>
       </c>
@@ -2243,7 +2242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:4">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B55" s="1">
         <v>2212</v>
       </c>
@@ -2254,7 +2253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:4">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B56" s="1">
         <v>2215</v>
       </c>
@@ -2265,7 +2264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:4">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B57" s="1">
         <v>2216</v>
       </c>
@@ -2276,7 +2275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:4">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B58" s="1">
         <v>2219</v>
       </c>
@@ -2287,7 +2286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:4">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B59" s="1">
         <v>2222</v>
       </c>
@@ -2298,7 +2297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:4">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B60" s="1">
         <v>2224</v>
       </c>
@@ -2309,7 +2308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:4">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B61" s="1">
         <v>2226</v>
       </c>
@@ -2320,7 +2319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="2:4">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B62" s="1">
         <v>2230</v>
       </c>
@@ -2331,7 +2330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:4">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B63" s="1">
         <v>2233</v>
       </c>
@@ -2342,7 +2341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:4">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B64" s="1">
         <v>2236</v>
       </c>
@@ -2353,7 +2352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="2:4">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B65" s="1">
         <v>2239</v>
       </c>
@@ -2364,7 +2363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:4">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B66" s="1">
         <v>2240</v>
       </c>
@@ -2375,7 +2374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="2:4">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B67" s="1">
         <v>2242</v>
       </c>
@@ -2386,7 +2385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="2:4">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B68" s="1">
         <v>2243</v>
       </c>
@@ -2397,7 +2396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="2:4">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B69" s="1">
         <v>2244</v>
       </c>
@@ -2408,7 +2407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="2:4">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B70" s="1">
         <v>2246</v>
       </c>
@@ -2419,7 +2418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="2:4">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B71" s="1">
         <v>2247</v>
       </c>
@@ -2430,7 +2429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="2:4">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B72" s="1">
         <v>2248</v>
       </c>
@@ -2441,7 +2440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:4">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B73" s="1">
         <v>2251</v>
       </c>
@@ -2452,7 +2451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="2:4">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B74" s="1">
         <v>2254</v>
       </c>
@@ -2463,7 +2462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="2:4">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B75" s="1">
         <v>2257</v>
       </c>
@@ -2474,7 +2473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="2:4">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B76" s="1">
         <v>2260</v>
       </c>
@@ -2485,7 +2484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="2:4">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B77" s="1">
         <v>2263</v>
       </c>
@@ -2496,7 +2495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="2:4">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B78" s="1">
         <v>2265</v>
       </c>
@@ -2507,7 +2506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="2:4">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B79" s="1">
         <v>2268</v>
       </c>
@@ -2518,7 +2517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="2:4">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B80" s="1">
         <v>2270</v>
       </c>
@@ -2529,7 +2528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="2:4">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B81" s="1">
         <v>2272</v>
       </c>
@@ -2540,7 +2539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="2:4">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B82" s="1">
         <v>2275</v>
       </c>
@@ -2551,7 +2550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="2:4">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B83" s="1">
         <v>2277</v>
       </c>
@@ -2562,7 +2561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="2:4">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B84" s="1">
         <v>2279</v>
       </c>
@@ -2573,7 +2572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="2:4">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B85" s="1">
         <v>2281</v>
       </c>
@@ -2584,7 +2583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="2:4">
+    <row r="86" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B86" s="1">
         <v>2284</v>
       </c>
@@ -2595,7 +2594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="2:4">
+    <row r="87" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B87" s="1">
         <v>2286</v>
       </c>
@@ -2606,7 +2605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="2:4">
+    <row r="88" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B88" s="1">
         <v>2288</v>
       </c>
@@ -2617,7 +2616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="2:4">
+    <row r="89" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B89" s="1">
         <v>2290</v>
       </c>
@@ -2628,7 +2627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="2:4">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B90" s="1">
         <v>2292</v>
       </c>
@@ -2639,7 +2638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="2:4">
+    <row r="91" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B91" s="1">
         <v>2294</v>
       </c>
@@ -2650,7 +2649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="2:4">
+    <row r="92" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B92" s="1">
         <v>2296</v>
       </c>
@@ -2661,7 +2660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="2:4">
+    <row r="93" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B93" s="1">
         <v>2297</v>
       </c>
@@ -2672,7 +2671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="2:4">
+    <row r="94" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B94" s="1">
         <v>2298</v>
       </c>
@@ -2683,7 +2682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="2:4">
+    <row r="95" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B95" s="1">
         <v>2299</v>
       </c>
@@ -2694,7 +2693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="2:4">
+    <row r="96" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B96" s="1">
         <v>2302</v>
       </c>
@@ -2705,7 +2704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="2:4">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B97" s="1">
         <v>2305</v>
       </c>
@@ -2716,7 +2715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="2:4">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B98" s="1">
         <v>2309</v>
       </c>
@@ -2727,7 +2726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="2:4">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B99" s="1">
         <v>2312</v>
       </c>
@@ -2738,7 +2737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="2:4">
+    <row r="100" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B100" s="1">
         <v>2314</v>
       </c>
@@ -2749,7 +2748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="2:4">
+    <row r="101" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B101" s="1">
         <v>2317</v>
       </c>
@@ -2760,7 +2759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="2:4">
+    <row r="102" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B102" s="1">
         <v>2320</v>
       </c>
@@ -2771,7 +2770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="2:4">
+    <row r="103" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B103" s="1">
         <v>2323</v>
       </c>
@@ -2782,7 +2781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="2:4">
+    <row r="104" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B104" s="1">
         <v>2327</v>
       </c>
@@ -2793,7 +2792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="2:4">
+    <row r="105" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B105" s="1">
         <v>2329</v>
       </c>
@@ -2804,7 +2803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="2:4">
+    <row r="106" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B106" s="1">
         <v>2331</v>
       </c>
@@ -2815,7 +2814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="2:4">
+    <row r="107" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B107" s="1">
         <v>2334</v>
       </c>
@@ -2826,7 +2825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="2:4">
+    <row r="108" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B108" s="1">
         <v>2336</v>
       </c>
@@ -2837,7 +2836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="2:4">
+    <row r="109" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B109" s="1">
         <v>2338</v>
       </c>
@@ -2848,7 +2847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="2:4">
+    <row r="110" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B110" s="1">
         <v>2340</v>
       </c>
@@ -2859,7 +2858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="2:4">
+    <row r="111" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B111" s="1">
         <v>2342</v>
       </c>
@@ -2870,7 +2869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="2:4">
+    <row r="112" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B112" s="1">
         <v>2344</v>
       </c>
@@ -2881,7 +2880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="2:4">
+    <row r="113" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B113" s="1">
         <v>2356</v>
       </c>
@@ -2892,7 +2891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="2:4">
+    <row r="114" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B114" s="1">
         <v>2358</v>
       </c>
@@ -2903,7 +2902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="2:4">
+    <row r="115" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B115" s="1">
         <v>2360</v>
       </c>
@@ -2914,7 +2913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="2:4">
+    <row r="116" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B116" s="1">
         <v>2362</v>
       </c>
@@ -2925,7 +2924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="2:4">
+    <row r="117" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B117" s="1">
         <v>2364</v>
       </c>
@@ -2936,7 +2935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="2:4">
+    <row r="118" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B118" s="1">
         <v>2367</v>
       </c>
@@ -2947,7 +2946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="2:4">
+    <row r="119" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B119" s="1">
         <v>2370</v>
       </c>
@@ -2958,7 +2957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="2:4">
+    <row r="120" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B120" s="1">
         <v>2384</v>
       </c>
@@ -2969,7 +2968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="2:4">
+    <row r="121" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B121" s="1">
         <v>2387</v>
       </c>
@@ -2980,7 +2979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="2:4">
+    <row r="122" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B122" s="1">
         <v>2469</v>
       </c>
@@ -2991,7 +2990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="2:4">
+    <row r="123" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B123" s="1">
         <v>2472</v>
       </c>
@@ -3002,7 +3001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="2:4">
+    <row r="124" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B124" s="1">
         <v>2475</v>
       </c>
@@ -3013,7 +3012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="2:4">
+    <row r="125" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B125" s="1">
         <v>2478</v>
       </c>
@@ -3024,7 +3023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="2:4">
+    <row r="126" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B126" s="1">
         <v>2532</v>
       </c>
@@ -3035,7 +3034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="2:4">
+    <row r="127" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B127" s="1">
         <v>2536</v>
       </c>
@@ -3046,7 +3045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="2:4">
+    <row r="128" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B128" s="1">
         <v>2540</v>
       </c>
@@ -3057,7 +3056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="2:4">
+    <row r="129" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B129" s="1">
         <v>2542</v>
       </c>
@@ -3068,7 +3067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="2:4">
+    <row r="130" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B130" s="1">
         <v>2545</v>
       </c>
@@ -3079,7 +3078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="2:4">
+    <row r="131" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B131" s="1">
         <v>2547</v>
       </c>
@@ -3090,7 +3089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="2:4">
+    <row r="132" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B132" s="1">
         <v>2549</v>
       </c>
@@ -3101,7 +3100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="2:4">
+    <row r="133" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B133" s="1">
         <v>2551</v>
       </c>
@@ -3112,7 +3111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="2:4">
+    <row r="134" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B134" s="1">
         <v>2553</v>
       </c>
@@ -3123,7 +3122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="2:4">
+    <row r="135" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B135" s="1">
         <v>2556</v>
       </c>
@@ -3134,7 +3133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="2:4">
+    <row r="136" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B136" s="1">
         <v>2568</v>
       </c>
@@ -3145,7 +3144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="2:4">
+    <row r="137" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B137" s="1">
         <v>2573</v>
       </c>
@@ -3156,7 +3155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="2:4">
+    <row r="138" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B138" s="1">
         <v>2579</v>
       </c>
@@ -3167,7 +3166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="2:4">
+    <row r="139" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B139" s="1">
         <v>2582</v>
       </c>
@@ -3178,7 +3177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="2:4">
+    <row r="140" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B140" s="1">
         <v>2585</v>
       </c>
@@ -3189,7 +3188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="2:4">
+    <row r="141" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B141" s="1">
         <v>2586</v>
       </c>
@@ -3200,7 +3199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="2:4">
+    <row r="142" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B142" s="1">
         <v>2589</v>
       </c>
@@ -3211,7 +3210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="2:4">
+    <row r="143" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B143" s="1">
         <v>2593</v>
       </c>
@@ -3222,7 +3221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="2:4">
+    <row r="144" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B144" s="1">
         <v>2598</v>
       </c>
@@ -3233,7 +3232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="2:4">
+    <row r="145" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B145" s="1">
         <v>2603</v>
       </c>
@@ -3244,7 +3243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="2:4">
+    <row r="146" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B146" s="1">
         <v>2608</v>
       </c>
@@ -3255,7 +3254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="2:4">
+    <row r="147" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B147" s="1">
         <v>2614</v>
       </c>
@@ -3266,7 +3265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="2:4">
+    <row r="148" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B148" s="1">
         <v>2618</v>
       </c>
@@ -3277,7 +3276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="2:4">
+    <row r="149" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B149" s="1">
         <v>2621</v>
       </c>
@@ -3288,7 +3287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="2:4">
+    <row r="150" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B150" s="1">
         <v>2626</v>
       </c>
@@ -3299,7 +3298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="2:4">
+    <row r="151" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B151" s="1">
         <v>2631</v>
       </c>
@@ -3310,7 +3309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="2:4">
+    <row r="152" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B152" s="1">
         <v>2636</v>
       </c>
@@ -3321,7 +3320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="2:4">
+    <row r="153" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B153" s="1">
         <v>2640</v>
       </c>
@@ -3329,7 +3328,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="154" spans="2:4">
+    <row r="154" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B154" s="1">
         <v>2645</v>
       </c>
@@ -3340,7 +3339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="2:4">
+    <row r="155" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B155" s="1">
         <v>2648</v>
       </c>
@@ -3351,7 +3350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="2:4">
+    <row r="156" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B156" s="1">
         <v>2680</v>
       </c>
@@ -3359,7 +3358,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="157" spans="2:4">
+    <row r="157" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B157" s="1">
         <v>2698</v>
       </c>
@@ -3370,7 +3369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="2:4">
+    <row r="158" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B158" s="1">
         <v>2704</v>
       </c>
@@ -3381,7 +3380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="2:4">
+    <row r="159" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B159" s="1">
         <v>3278</v>
       </c>
@@ -3389,7 +3388,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="160" spans="2:4">
+    <row r="160" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B160" s="1">
         <v>3280</v>
       </c>
@@ -3397,7 +3396,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="161" spans="2:3">
+    <row r="161" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B161" s="1">
         <v>3628</v>
       </c>
@@ -3405,7 +3404,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="162" spans="2:3">
+    <row r="162" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B162" s="1">
         <v>3631</v>
       </c>
@@ -3413,7 +3412,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="163" spans="2:3">
+    <row r="163" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B163" s="1">
         <v>3633</v>
       </c>
@@ -3421,7 +3420,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="164" spans="2:3">
+    <row r="164" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B164" s="1">
         <v>4791</v>
       </c>
@@ -3429,7 +3428,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="165" spans="2:3">
+    <row r="165" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B165" s="1">
         <v>81</v>
       </c>
@@ -3437,7 +3436,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="166" spans="2:3">
+    <row r="166" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B166" s="1">
         <v>82</v>
       </c>
@@ -3445,7 +3444,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="167" spans="2:3">
+    <row r="167" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B167" s="1">
         <v>83</v>
       </c>
@@ -3453,7 +3452,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="168" spans="2:3">
+    <row r="168" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B168" s="1">
         <v>84</v>
       </c>
@@ -3461,7 +3460,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="169" spans="2:3">
+    <row r="169" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B169" s="1">
         <v>85</v>
       </c>
@@ -3469,7 +3468,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="170" spans="2:3">
+    <row r="170" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B170" s="1">
         <v>89</v>
       </c>
@@ -3477,7 +3476,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="171" spans="2:3">
+    <row r="171" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B171" s="1">
         <v>90</v>
       </c>
@@ -3485,7 +3484,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="172" spans="2:3">
+    <row r="172" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B172" s="1">
         <v>110</v>
       </c>
@@ -3493,7 +3492,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="173" spans="2:3">
+    <row r="173" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B173" s="1">
         <v>111</v>
       </c>
@@ -3501,7 +3500,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="174" spans="2:3">
+    <row r="174" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B174" s="1">
         <v>112</v>
       </c>
@@ -3509,7 +3508,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="175" spans="2:3">
+    <row r="175" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B175" s="1">
         <v>113</v>
       </c>
@@ -3517,7 +3516,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="176" spans="2:3">
+    <row r="176" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B176" s="1">
         <v>115</v>
       </c>
@@ -3525,7 +3524,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="177" spans="2:4">
+    <row r="177" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B177" s="1">
         <v>116</v>
       </c>
@@ -3533,7 +3532,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="178" spans="2:4">
+    <row r="178" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B178" s="1">
         <v>117</v>
       </c>
@@ -3541,7 +3540,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="179" spans="2:4">
+    <row r="179" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B179" s="1">
         <v>118</v>
       </c>
@@ -3549,7 +3548,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="180" spans="2:4">
+    <row r="180" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B180" s="1">
         <v>143</v>
       </c>
@@ -3557,7 +3556,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="181" spans="2:4">
+    <row r="181" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B181" s="1">
         <v>370</v>
       </c>
@@ -3565,7 +3564,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="182" spans="2:4">
+    <row r="182" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B182" s="1">
         <v>412</v>
       </c>
@@ -3573,7 +3572,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="183" spans="2:4">
+    <row r="183" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B183" s="1">
         <v>453</v>
       </c>
@@ -3581,7 +3580,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="184" spans="2:4">
+    <row r="184" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B184" s="1">
         <v>602</v>
       </c>
@@ -3589,7 +3588,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="185" spans="2:4">
+    <row r="185" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B185" s="1">
         <v>698</v>
       </c>
@@ -3597,7 +3596,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="186" spans="2:4">
+    <row r="186" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B186" s="1">
         <v>734</v>
       </c>
@@ -3605,7 +3604,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="187" spans="2:4">
+    <row r="187" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B187" s="1">
         <v>777</v>
       </c>
@@ -3613,7 +3612,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="188" spans="2:4">
+    <row r="188" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B188" s="1">
         <v>816</v>
       </c>
@@ -3621,7 +3620,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="189" spans="2:4">
+    <row r="189" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B189" s="1">
         <v>851</v>
       </c>
@@ -3629,7 +3628,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="190" spans="2:4">
+    <row r="190" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B190" s="1">
         <v>912</v>
       </c>
@@ -3640,7 +3639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="2:4">
+    <row r="191" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B191" s="1">
         <v>940</v>
       </c>
@@ -3651,7 +3650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="2:4">
+    <row r="192" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B192" s="1">
         <v>978</v>
       </c>
@@ -3662,7 +3661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="2:4">
+    <row r="193" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B193" s="1">
         <v>1267</v>
       </c>
@@ -3670,7 +3669,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="194" spans="2:4">
+    <row r="194" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B194" s="1">
         <v>1311</v>
       </c>
@@ -3681,7 +3680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="2:4">
+    <row r="195" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B195" s="1">
         <v>1399</v>
       </c>
@@ -3692,7 +3691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="2:4">
+    <row r="196" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B196" s="1">
         <v>1465</v>
       </c>
@@ -3700,7 +3699,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="197" spans="2:4">
+    <row r="197" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B197" s="1">
         <v>1687</v>
       </c>
@@ -3711,7 +3710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="2:4">
+    <row r="198" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B198" s="1">
         <v>2018</v>
       </c>
@@ -3722,7 +3721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="2:4">
+    <row r="199" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B199" s="1">
         <v>2057</v>
       </c>
@@ -3730,7 +3729,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="200" spans="2:4">
+    <row r="200" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B200" s="1">
         <v>2090</v>
       </c>
@@ -3741,7 +3740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="2:4">
+    <row r="201" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B201" s="1">
         <v>2444</v>
       </c>
@@ -3752,7 +3751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="2:4">
+    <row r="202" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B202" s="1">
         <v>2495</v>
       </c>
@@ -3763,7 +3762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="2:4">
+    <row r="203" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B203" s="1">
         <v>2656</v>
       </c>
@@ -3771,7 +3770,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="204" spans="2:4">
+    <row r="204" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B204" s="1">
         <v>2755</v>
       </c>
@@ -3779,7 +3778,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="205" spans="2:4">
+    <row r="205" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B205" s="1">
         <v>2926</v>
       </c>
@@ -3787,7 +3786,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="206" spans="2:4">
+    <row r="206" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B206" s="1">
         <v>2987</v>
       </c>
@@ -3795,7 +3794,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="207" spans="2:4">
+    <row r="207" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B207" s="1">
         <v>3038</v>
       </c>
@@ -3803,7 +3802,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="208" spans="2:4">
+    <row r="208" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B208" s="1">
         <v>3079</v>
       </c>
@@ -3811,7 +3810,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="209" spans="2:3">
+    <row r="209" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B209" s="1">
         <v>3094</v>
       </c>
@@ -3819,7 +3818,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="210" spans="2:3">
+    <row r="210" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B210" s="1">
         <v>3109</v>
       </c>
@@ -3827,7 +3826,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="211" spans="2:3">
+    <row r="211" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B211" s="1">
         <v>3120</v>
       </c>
@@ -3835,7 +3834,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="212" spans="2:3">
+    <row r="212" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B212" s="1">
         <v>3155</v>
       </c>
@@ -3843,7 +3842,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="213" spans="2:3">
+    <row r="213" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B213" s="1">
         <v>3238</v>
       </c>
@@ -3851,7 +3850,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="214" spans="2:3">
+    <row r="214" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B214" s="1">
         <v>3285</v>
       </c>
@@ -3859,7 +3858,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="215" spans="2:3">
+    <row r="215" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B215" s="1">
         <v>3286</v>
       </c>
@@ -3867,7 +3866,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="216" spans="2:3">
+    <row r="216" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B216" s="1">
         <v>3287</v>
       </c>
@@ -3875,7 +3874,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="217" spans="2:3">
+    <row r="217" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B217" s="1">
         <v>3288</v>
       </c>
@@ -3883,7 +3882,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="218" spans="2:3">
+    <row r="218" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B218" s="1">
         <v>3375</v>
       </c>
@@ -3891,7 +3890,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="219" spans="2:3">
+    <row r="219" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B219" s="1">
         <v>3647</v>
       </c>
@@ -3899,7 +3898,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="220" spans="2:3">
+    <row r="220" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B220" s="1">
         <v>3688</v>
       </c>
@@ -3907,7 +3906,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="221" spans="2:3">
+    <row r="221" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B221" s="1">
         <v>3726</v>
       </c>
@@ -3915,7 +3914,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="222" spans="2:3">
+    <row r="222" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B222" s="1">
         <v>3800</v>
       </c>
@@ -3923,7 +3922,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="223" spans="2:3">
+    <row r="223" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B223" s="1">
         <v>3830</v>
       </c>
@@ -3931,7 +3930,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="224" spans="2:3">
+    <row r="224" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B224" s="1">
         <v>3880</v>
       </c>
@@ -3939,7 +3938,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="225" spans="2:4">
+    <row r="225" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B225" s="1">
         <v>4039</v>
       </c>
@@ -3947,7 +3946,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="226" spans="2:4">
+    <row r="226" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B226" s="1">
         <v>4118</v>
       </c>
@@ -3955,7 +3954,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="227" spans="2:4">
+    <row r="227" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B227" s="1">
         <v>4106</v>
       </c>
@@ -3963,7 +3962,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="228" spans="2:4">
+    <row r="228" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B228" s="1">
         <v>4248</v>
       </c>
@@ -3971,7 +3970,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="229" spans="2:4">
+    <row r="229" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B229" s="1">
         <v>4262</v>
       </c>
@@ -3979,7 +3978,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="230" spans="2:4">
+    <row r="230" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B230" s="1">
         <v>4345</v>
       </c>
@@ -3987,7 +3986,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="231" spans="2:4">
+    <row r="231" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B231" s="1">
         <v>4389</v>
       </c>
@@ -3995,7 +3994,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="232" spans="2:4">
+    <row r="232" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B232" s="1">
         <v>4464</v>
       </c>
@@ -4006,7 +4005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="2:4">
+    <row r="233" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B233" s="1">
         <v>4714</v>
       </c>
@@ -4014,7 +4013,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="234" spans="2:4">
+    <row r="234" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B234" s="1">
         <v>4784</v>
       </c>
@@ -4022,7 +4021,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="235" spans="2:4">
+    <row r="235" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B235" s="1">
         <v>4795</v>
       </c>
@@ -4030,7 +4029,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="236" spans="2:4">
+    <row r="236" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B236" s="1">
         <v>4812</v>
       </c>
@@ -4038,7 +4037,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="237" spans="2:4">
+    <row r="237" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B237" s="1">
         <v>4824</v>
       </c>
@@ -4046,7 +4045,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="238" spans="2:4">
+    <row r="238" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B238" s="1">
         <v>4839</v>
       </c>
@@ -4057,7 +4056,7 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="B2:D238">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4070,22 +4069,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:D128"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:D127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C112" sqref="C112"/>
+      <selection pane="bottomLeft" activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="7.625" style="1" customWidth="1"/>
     <col min="3" max="3" width="84" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
         <v>163</v>
       </c>
@@ -4096,7 +4095,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B2" s="1">
         <v>69</v>
       </c>
@@ -4104,7 +4103,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B3" s="1">
         <v>80</v>
       </c>
@@ -4112,7 +4111,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B4" s="1">
         <v>107</v>
       </c>
@@ -4120,7 +4119,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B5" s="1">
         <v>133</v>
       </c>
@@ -4128,7 +4127,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B6" s="1">
         <v>222</v>
       </c>
@@ -4136,7 +4135,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B7" s="1">
         <v>290</v>
       </c>
@@ -4144,7 +4143,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B8" s="1">
         <v>293</v>
       </c>
@@ -4152,7 +4151,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B9" s="1">
         <v>298</v>
       </c>
@@ -4160,7 +4159,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B10" s="1">
         <v>304</v>
       </c>
@@ -4168,7 +4167,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B11" s="1">
         <v>310</v>
       </c>
@@ -4176,7 +4175,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B12" s="1">
         <v>318</v>
       </c>
@@ -4184,7 +4183,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B13" s="1">
         <v>324</v>
       </c>
@@ -4192,7 +4191,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="14" spans="2:4">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B14" s="1">
         <v>327</v>
       </c>
@@ -4200,7 +4199,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="15" spans="2:4">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B15" s="1">
         <v>331</v>
       </c>
@@ -4208,7 +4207,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="16" spans="2:4">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B16" s="1">
         <v>335</v>
       </c>
@@ -4216,7 +4215,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B17" s="1">
         <v>339</v>
       </c>
@@ -4224,7 +4223,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B18" s="1">
         <v>342</v>
       </c>
@@ -4232,7 +4231,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B19" s="1">
         <v>346</v>
       </c>
@@ -4240,7 +4239,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B20" s="1">
         <v>352</v>
       </c>
@@ -4251,7 +4250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B21" s="1">
         <v>362</v>
       </c>
@@ -4259,7 +4258,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="22" spans="2:4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B22" s="1">
         <v>364</v>
       </c>
@@ -4267,7 +4266,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B23" s="1">
         <v>366</v>
       </c>
@@ -4275,7 +4274,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B24" s="1">
         <v>373</v>
       </c>
@@ -4283,7 +4282,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="25" spans="2:4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B25" s="1">
         <v>381</v>
       </c>
@@ -4294,7 +4293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:4">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B26" s="1">
         <v>386</v>
       </c>
@@ -4305,7 +4304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:4">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B27" s="1">
         <v>391</v>
       </c>
@@ -4316,7 +4315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:4">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B28" s="1">
         <v>393</v>
       </c>
@@ -4327,7 +4326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:4">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B29" s="1">
         <v>398</v>
       </c>
@@ -4338,7 +4337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:4">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B30" s="1">
         <v>402</v>
       </c>
@@ -4349,7 +4348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:4">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B31" s="1">
         <v>406</v>
       </c>
@@ -4360,7 +4359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:4">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B32" s="1">
         <v>411</v>
       </c>
@@ -4371,7 +4370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:4">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B33" s="1">
         <v>416</v>
       </c>
@@ -4382,7 +4381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:4">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B34" s="1">
         <v>421</v>
       </c>
@@ -4393,7 +4392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:4">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B35" s="1">
         <v>427</v>
       </c>
@@ -4404,7 +4403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:4">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B36" s="1">
         <v>433</v>
       </c>
@@ -4415,7 +4414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:4">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B37" s="1">
         <v>438</v>
       </c>
@@ -4426,7 +4425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:4">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B38" s="1">
         <v>443</v>
       </c>
@@ -4437,7 +4436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:4">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B39" s="1">
         <v>448</v>
       </c>
@@ -4448,7 +4447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:4">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B40" s="1">
         <v>453</v>
       </c>
@@ -4459,7 +4458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:4">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B41" s="1">
         <v>458</v>
       </c>
@@ -4470,7 +4469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:4">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B42" s="1">
         <v>461</v>
       </c>
@@ -4481,7 +4480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:4">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B43" s="1">
         <v>466</v>
       </c>
@@ -4492,7 +4491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:4">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B44" s="1">
         <v>470</v>
       </c>
@@ -4503,7 +4502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:4">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B45" s="1">
         <v>475</v>
       </c>
@@ -4514,7 +4513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:4">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B46" s="1">
         <v>481</v>
       </c>
@@ -4525,7 +4524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:4">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B47" s="1">
         <v>486</v>
       </c>
@@ -4536,7 +4535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:4">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B48" s="1">
         <v>491</v>
       </c>
@@ -4547,7 +4546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:4">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B49" s="1">
         <v>506</v>
       </c>
@@ -4555,7 +4554,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="50" spans="2:4">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B50" s="1">
         <v>533</v>
       </c>
@@ -4566,7 +4565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:4">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B51" s="1">
         <v>539</v>
       </c>
@@ -4577,7 +4576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:4">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B52" s="1">
         <v>545</v>
       </c>
@@ -4588,7 +4587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:4">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B53" s="1">
         <v>564</v>
       </c>
@@ -4599,7 +4598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:4">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B54" s="1">
         <v>569</v>
       </c>
@@ -4610,7 +4609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:4">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B55" s="1">
         <v>576</v>
       </c>
@@ -4621,7 +4620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:4">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B56" s="1">
         <v>590</v>
       </c>
@@ -4632,7 +4631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:4">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B57" s="1">
         <v>596</v>
       </c>
@@ -4643,7 +4642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:4">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B58" s="1">
         <v>601</v>
       </c>
@@ -4654,7 +4653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:4">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B59" s="1">
         <v>603</v>
       </c>
@@ -4665,7 +4664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:4">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B60" s="1">
         <v>605</v>
       </c>
@@ -4676,7 +4675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:4">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B61" s="1">
         <v>607</v>
       </c>
@@ -4687,7 +4686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="2:4">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B62" s="1">
         <v>609</v>
       </c>
@@ -4698,7 +4697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:4">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B63" s="1">
         <v>610</v>
       </c>
@@ -4709,7 +4708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:4">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B64" s="1">
         <v>613</v>
       </c>
@@ -4720,7 +4719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="2:4">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B65" s="1">
         <v>617</v>
       </c>
@@ -4731,7 +4730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:4">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B66" s="1">
         <v>620</v>
       </c>
@@ -4742,7 +4741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="2:4">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B67" s="1">
         <v>623</v>
       </c>
@@ -4753,7 +4752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="2:4">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B68" s="1">
         <v>628</v>
       </c>
@@ -4764,7 +4763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="2:4">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B69" s="1">
         <v>631</v>
       </c>
@@ -4775,7 +4774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="2:4">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B70" s="1">
         <v>634</v>
       </c>
@@ -4786,7 +4785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="2:4">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B71" s="1">
         <v>637</v>
       </c>
@@ -4797,7 +4796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="2:4">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B72" s="1">
         <v>641</v>
       </c>
@@ -4808,7 +4807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:4">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B73" s="1">
         <v>643</v>
       </c>
@@ -4819,7 +4818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="2:4">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B74" s="1">
         <v>645</v>
       </c>
@@ -4830,7 +4829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="2:4">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B75" s="1">
         <v>647</v>
       </c>
@@ -4841,7 +4840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="2:4">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B76" s="1">
         <v>656</v>
       </c>
@@ -4852,7 +4851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="2:4">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B77" s="1">
         <v>663</v>
       </c>
@@ -4863,7 +4862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="2:4">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B78" s="1">
         <v>668</v>
       </c>
@@ -4874,7 +4873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="2:4">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B79" s="1">
         <v>671</v>
       </c>
@@ -4885,7 +4884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="2:4" s="1" customFormat="1">
+    <row r="80" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B80" s="1">
         <v>675</v>
       </c>
@@ -4896,7 +4895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="2:4" s="1" customFormat="1">
+    <row r="81" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B81" s="1">
         <v>679</v>
       </c>
@@ -4907,7 +4906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="2:4" s="1" customFormat="1">
+    <row r="82" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B82" s="1">
         <v>685</v>
       </c>
@@ -4918,7 +4917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="2:4" s="1" customFormat="1">
+    <row r="83" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B83" s="1">
         <v>696</v>
       </c>
@@ -4929,7 +4928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="2:4" s="1" customFormat="1">
+    <row r="84" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B84" s="1">
         <v>702</v>
       </c>
@@ -4940,7 +4939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="2:4" s="1" customFormat="1">
+    <row r="85" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B85" s="1">
         <v>706</v>
       </c>
@@ -4951,7 +4950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="2:4" s="1" customFormat="1">
+    <row r="86" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B86" s="1">
         <v>713</v>
       </c>
@@ -4962,7 +4961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="2:4" s="1" customFormat="1">
+    <row r="87" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B87" s="1">
         <v>719</v>
       </c>
@@ -4970,7 +4969,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="88" spans="2:4" s="1" customFormat="1">
+    <row r="88" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B88" s="1">
         <v>725</v>
       </c>
@@ -4978,7 +4977,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="89" spans="2:4" s="1" customFormat="1">
+    <row r="89" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B89" s="1">
         <v>733</v>
       </c>
@@ -4989,7 +4988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="2:4" s="1" customFormat="1">
+    <row r="90" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B90" s="1">
         <v>739</v>
       </c>
@@ -4997,7 +4996,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="91" spans="2:4" s="1" customFormat="1">
+    <row r="91" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B91" s="1">
         <v>744</v>
       </c>
@@ -5005,7 +5004,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="92" spans="2:4" s="1" customFormat="1">
+    <row r="92" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B92" s="1">
         <v>758</v>
       </c>
@@ -5016,7 +5015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="2:4" s="1" customFormat="1">
+    <row r="93" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B93" s="1">
         <v>761</v>
       </c>
@@ -5024,7 +5023,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="94" spans="2:4" s="1" customFormat="1">
+    <row r="94" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B94" s="1">
         <v>764</v>
       </c>
@@ -5035,7 +5034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="2:4" s="1" customFormat="1">
+    <row r="95" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B95" s="1">
         <v>766</v>
       </c>
@@ -5043,7 +5042,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="96" spans="2:4" s="1" customFormat="1">
+    <row r="96" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B96" s="1">
         <v>779</v>
       </c>
@@ -5051,7 +5050,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="97" spans="2:4" s="1" customFormat="1">
+    <row r="97" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B97" s="1">
         <v>781</v>
       </c>
@@ -5062,7 +5061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="2:4" s="1" customFormat="1">
+    <row r="98" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B98" s="1">
         <v>786</v>
       </c>
@@ -5073,7 +5072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="2:4" s="1" customFormat="1">
+    <row r="99" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B99" s="1">
         <v>789</v>
       </c>
@@ -5084,7 +5083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="2:4" s="1" customFormat="1">
+    <row r="100" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B100" s="1">
         <v>812</v>
       </c>
@@ -5095,7 +5094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="2:4" s="1" customFormat="1">
+    <row r="101" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B101" s="1">
         <v>823</v>
       </c>
@@ -5106,7 +5105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="2:4" s="1" customFormat="1">
+    <row r="102" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B102" s="1">
         <v>828</v>
       </c>
@@ -5117,7 +5116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="2:4" s="1" customFormat="1">
+    <row r="103" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B103" s="1">
         <v>834</v>
       </c>
@@ -5128,7 +5127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="2:4" s="1" customFormat="1">
+    <row r="104" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B104" s="1">
         <v>840</v>
       </c>
@@ -5139,7 +5138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="2:4" s="1" customFormat="1">
+    <row r="105" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B105" s="1">
         <v>1091</v>
       </c>
@@ -5150,197 +5149,252 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="2:4" s="1" customFormat="1">
+    <row r="106" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B106" s="1">
         <v>1094</v>
       </c>
       <c r="C106" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="107" spans="2:4" s="1" customFormat="1">
+      <c r="D106" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B107" s="1">
         <v>1116</v>
       </c>
       <c r="C107" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="108" spans="2:4" s="1" customFormat="1">
+      <c r="D107" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B108" s="1">
         <v>1119</v>
       </c>
       <c r="C108" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="109" spans="2:4">
+      <c r="D108" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B109" s="1">
-        <v>1120</v>
+        <v>1126</v>
       </c>
       <c r="C109" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="110" spans="2:4">
+      <c r="D109" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B110" s="1">
-        <v>1126</v>
+        <v>1149</v>
       </c>
       <c r="C110" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="111" spans="2:4">
+      <c r="D110" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B111" s="1">
-        <v>1149</v>
+        <v>1154</v>
       </c>
       <c r="C111" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="112" spans="2:4">
+        <v>350</v>
+      </c>
+      <c r="D111" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B112" s="1">
-        <v>1154</v>
+        <v>1158</v>
       </c>
       <c r="C112" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="113" spans="2:4">
+      <c r="D112" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B113" s="1">
-        <v>1158</v>
+        <v>1165</v>
       </c>
       <c r="C113" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="114" spans="2:4">
+      <c r="D113" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B114" s="1">
-        <v>1165</v>
+        <v>1170</v>
       </c>
       <c r="C114" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="115" spans="2:4">
+      <c r="D114" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B115" s="1">
-        <v>1170</v>
+        <v>1172</v>
       </c>
       <c r="C115" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="116" spans="2:4">
+      <c r="D115" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B116" s="1">
-        <v>1172</v>
+        <v>1174</v>
       </c>
       <c r="C116" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="117" spans="2:4">
+      <c r="D116" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B117" s="1">
-        <v>1174</v>
+        <v>1176</v>
       </c>
       <c r="C117" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="118" spans="2:4">
+      <c r="D117" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B118" s="1">
-        <v>1176</v>
+        <v>1178</v>
       </c>
       <c r="C118" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="119" spans="2:4">
+      <c r="D118" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B119" s="1">
-        <v>1178</v>
+        <v>1181</v>
       </c>
       <c r="C119" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="120" spans="2:4">
+      <c r="D119" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B120" s="1">
-        <v>1181</v>
+        <v>1184</v>
       </c>
       <c r="C120" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="121" spans="2:4">
+      <c r="D120" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B121" s="1">
-        <v>1184</v>
+        <v>1187</v>
       </c>
       <c r="C121" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="122" spans="2:4">
+      <c r="D121" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B122" s="1">
-        <v>1187</v>
+        <v>1190</v>
       </c>
       <c r="C122" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="123" spans="2:4">
+      <c r="D122" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B123" s="1">
-        <v>1190</v>
+        <v>1193</v>
       </c>
       <c r="C123" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="124" spans="2:4">
+      <c r="D123" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B124" s="1">
-        <v>1193</v>
+        <v>1197</v>
       </c>
       <c r="C124" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="125" spans="2:4">
+      <c r="D124" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B125" s="1">
-        <v>1197</v>
+        <v>1200</v>
       </c>
       <c r="C125" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="126" spans="2:4">
+      <c r="D125" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B126" s="1">
-        <v>1200</v>
+        <v>1203</v>
       </c>
       <c r="C126" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="127" spans="2:4">
+      <c r="D126" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B127" s="1">
-        <v>1203</v>
+        <v>1206</v>
       </c>
       <c r="C127" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="128" spans="2:4">
-      <c r="B128" s="1">
-        <v>1206</v>
-      </c>
-      <c r="C128" t="s">
-        <v>367</v>
-      </c>
-      <c r="D128" s="1">
+      <c r="D127" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="B2:D128">
-    <cfRule type="expression" dxfId="2" priority="1">
+  <conditionalFormatting sqref="B2:D127">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>